<commit_message>
Inicio da implementação do leitor de arquivo com o novo padrão de malha
</commit_message>
<xml_diff>
--- a/malhas/malhas-mao-dupla.xlsx
+++ b/malhas/malhas-mao-dupla.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
-    <sheet name="malha-exemplo1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
+    <sheet name="malha-exemplo1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="29">
   <si>
     <t>→</t>
   </si>
@@ -56,12 +57,66 @@
   <si>
     <t>Colorir de acordo com o mapa</t>
   </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Codificação</t>
+  </si>
+  <si>
+    <t>Vazio</t>
+  </si>
+  <si>
+    <t>Cima</t>
+  </si>
+  <si>
+    <t>Direita</t>
+  </si>
+  <si>
+    <t>Baixo</t>
+  </si>
+  <si>
+    <t>Esquerda</t>
+  </si>
+  <si>
+    <t>Cima e Direita</t>
+  </si>
+  <si>
+    <t>Cima e Esquerda</t>
+  </si>
+  <si>
+    <t>Direita e Baixo</t>
+  </si>
+  <si>
+    <t>Cima e Baixo</t>
+  </si>
+  <si>
+    <t>Direita e Esquerda</t>
+  </si>
+  <si>
+    <t>Baixo e Esquerda</t>
+  </si>
+  <si>
+    <t>Cima, Direita e Baixo</t>
+  </si>
+  <si>
+    <t>Cima, Direita e Esquerda</t>
+  </si>
+  <si>
+    <t>Cima, Baixo e Esquerda</t>
+  </si>
+  <si>
+    <t>Direita, Baixo e Esquerda</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +140,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -156,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -183,6 +253,41 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,20 +598,3347 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF29"/>
+  <dimension ref="A1:BD29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG14" sqref="AG14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="26" width="2.7109375" customWidth="1"/>
-    <col min="27" max="27" width="5.7109375" customWidth="1"/>
-    <col min="28" max="31" width="4.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="7" width="2.28515625" customWidth="1"/>
+    <col min="8" max="9" width="2.42578125" customWidth="1"/>
+    <col min="10" max="10" width="2.5703125" customWidth="1"/>
+    <col min="11" max="11" width="2.7109375" customWidth="1"/>
+    <col min="12" max="12" width="3" customWidth="1"/>
+    <col min="13" max="13" width="2.5703125" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" customWidth="1"/>
+    <col min="15" max="29" width="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="56" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1">
+        <v>3</v>
+      </c>
+      <c r="I3" s="1">
+        <v>4</v>
+      </c>
+      <c r="J3" s="1">
+        <v>5</v>
+      </c>
+      <c r="K3" s="1">
+        <v>6</v>
+      </c>
+      <c r="L3" s="1">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>8</v>
+      </c>
+      <c r="N3" s="1">
+        <v>9</v>
+      </c>
+      <c r="O3" s="1">
+        <v>10</v>
+      </c>
+      <c r="P3" s="1">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>12</v>
+      </c>
+      <c r="R3" s="1">
+        <v>13</v>
+      </c>
+      <c r="S3" s="1">
+        <v>14</v>
+      </c>
+      <c r="T3" s="1">
+        <v>15</v>
+      </c>
+      <c r="U3" s="1">
+        <v>16</v>
+      </c>
+      <c r="V3" s="1">
+        <v>17</v>
+      </c>
+      <c r="W3" s="1">
+        <v>18</v>
+      </c>
+      <c r="X3" s="1">
+        <v>19</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>20</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>21</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>22</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>23</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>24</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AI3" s="1">
+        <v>3</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>4</v>
+      </c>
+      <c r="AK3" s="1">
+        <v>5</v>
+      </c>
+      <c r="AL3" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM3" s="1">
+        <v>7</v>
+      </c>
+      <c r="AN3" s="1">
+        <v>8</v>
+      </c>
+      <c r="AO3" s="1">
+        <v>9</v>
+      </c>
+      <c r="AP3" s="1">
+        <v>10</v>
+      </c>
+      <c r="AQ3" s="1">
+        <v>11</v>
+      </c>
+      <c r="AR3" s="1">
+        <v>12</v>
+      </c>
+      <c r="AS3" s="1">
+        <v>13</v>
+      </c>
+      <c r="AT3" s="1">
+        <v>14</v>
+      </c>
+      <c r="AU3" s="1">
+        <v>15</v>
+      </c>
+      <c r="AV3" s="1">
+        <v>16</v>
+      </c>
+      <c r="AW3" s="1">
+        <v>17</v>
+      </c>
+      <c r="AX3" s="1">
+        <v>18</v>
+      </c>
+      <c r="AY3" s="1">
+        <v>19</v>
+      </c>
+      <c r="AZ3" s="1">
+        <v>20</v>
+      </c>
+      <c r="BA3" s="1">
+        <v>21</v>
+      </c>
+      <c r="BB3" s="1">
+        <v>22</v>
+      </c>
+      <c r="BC3" s="1">
+        <v>23</v>
+      </c>
+      <c r="BD3" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="24">
+        <v>0</v>
+      </c>
+      <c r="F4" s="24">
+        <v>0</v>
+      </c>
+      <c r="G4" s="24">
+        <v>0</v>
+      </c>
+      <c r="H4" s="24">
+        <v>0</v>
+      </c>
+      <c r="I4" s="24">
+        <v>0</v>
+      </c>
+      <c r="J4" s="24">
+        <v>0</v>
+      </c>
+      <c r="K4" s="24">
+        <v>0</v>
+      </c>
+      <c r="L4" s="32">
+        <v>0</v>
+      </c>
+      <c r="M4" s="24">
+        <v>0</v>
+      </c>
+      <c r="N4" s="24">
+        <v>0</v>
+      </c>
+      <c r="O4" s="24">
+        <v>0</v>
+      </c>
+      <c r="P4" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="26">
+        <v>1</v>
+      </c>
+      <c r="R4" s="24">
+        <v>0</v>
+      </c>
+      <c r="S4" s="24">
+        <v>0</v>
+      </c>
+      <c r="T4" s="24">
+        <v>0</v>
+      </c>
+      <c r="U4" s="24">
+        <v>0</v>
+      </c>
+      <c r="V4" s="24">
+        <v>0</v>
+      </c>
+      <c r="W4" s="24">
+        <v>0</v>
+      </c>
+      <c r="X4" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="24">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="24">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="8"/>
+      <c r="AN4" s="8"/>
+      <c r="AO4" s="8"/>
+      <c r="AP4" s="8"/>
+      <c r="AQ4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS4" s="2"/>
+      <c r="AT4" s="2"/>
+      <c r="AU4" s="2"/>
+      <c r="AV4" s="2"/>
+      <c r="AW4" s="2"/>
+      <c r="AX4" s="2"/>
+      <c r="AY4" s="8"/>
+      <c r="AZ4" s="8"/>
+      <c r="BA4" s="8"/>
+      <c r="BB4" s="8"/>
+      <c r="BC4" s="8"/>
+      <c r="BD4" s="8"/>
+    </row>
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="24">
+        <v>0</v>
+      </c>
+      <c r="F5" s="24">
+        <v>0</v>
+      </c>
+      <c r="G5" s="24">
+        <v>0</v>
+      </c>
+      <c r="H5" s="24">
+        <v>0</v>
+      </c>
+      <c r="I5" s="24">
+        <v>0</v>
+      </c>
+      <c r="J5" s="24">
+        <v>0</v>
+      </c>
+      <c r="K5" s="32">
+        <v>0</v>
+      </c>
+      <c r="L5" s="24">
+        <v>0</v>
+      </c>
+      <c r="M5" s="24">
+        <v>0</v>
+      </c>
+      <c r="N5" s="24">
+        <v>0</v>
+      </c>
+      <c r="O5" s="24">
+        <v>0</v>
+      </c>
+      <c r="P5" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="26">
+        <v>1</v>
+      </c>
+      <c r="R5" s="24">
+        <v>0</v>
+      </c>
+      <c r="S5" s="24">
+        <v>0</v>
+      </c>
+      <c r="T5" s="24">
+        <v>0</v>
+      </c>
+      <c r="U5" s="24">
+        <v>0</v>
+      </c>
+      <c r="V5" s="24">
+        <v>0</v>
+      </c>
+      <c r="W5" s="24">
+        <v>0</v>
+      </c>
+      <c r="X5" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="24">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="24">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="8"/>
+      <c r="AN5" s="8"/>
+      <c r="AO5" s="8"/>
+      <c r="AP5" s="8"/>
+      <c r="AQ5" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS5" s="2"/>
+      <c r="AT5" s="2"/>
+      <c r="AU5" s="2"/>
+      <c r="AV5" s="2"/>
+      <c r="AW5" s="2"/>
+      <c r="AX5" s="2"/>
+      <c r="AY5" s="8"/>
+      <c r="AZ5" s="8"/>
+      <c r="BA5" s="8"/>
+      <c r="BB5" s="8"/>
+      <c r="BC5" s="8"/>
+      <c r="BD5" s="8"/>
+    </row>
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+      <c r="F6" s="24">
+        <v>0</v>
+      </c>
+      <c r="G6" s="24">
+        <v>0</v>
+      </c>
+      <c r="H6" s="24">
+        <v>0</v>
+      </c>
+      <c r="I6" s="24">
+        <v>0</v>
+      </c>
+      <c r="J6" s="24">
+        <v>0</v>
+      </c>
+      <c r="K6" s="24">
+        <v>0</v>
+      </c>
+      <c r="L6" s="24">
+        <v>0</v>
+      </c>
+      <c r="M6" s="24">
+        <v>0</v>
+      </c>
+      <c r="N6" s="24">
+        <v>0</v>
+      </c>
+      <c r="O6" s="24">
+        <v>0</v>
+      </c>
+      <c r="P6" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="26">
+        <v>1</v>
+      </c>
+      <c r="R6" s="24">
+        <v>0</v>
+      </c>
+      <c r="S6" s="24">
+        <v>0</v>
+      </c>
+      <c r="T6" s="24">
+        <v>0</v>
+      </c>
+      <c r="U6" s="24">
+        <v>0</v>
+      </c>
+      <c r="V6" s="24">
+        <v>0</v>
+      </c>
+      <c r="W6" s="24">
+        <v>0</v>
+      </c>
+      <c r="X6" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="24">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="24">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>2</v>
+      </c>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="8"/>
+      <c r="AN6" s="8"/>
+      <c r="AO6" s="8"/>
+      <c r="AP6" s="8"/>
+      <c r="AQ6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS6" s="2"/>
+      <c r="AT6" s="2"/>
+      <c r="AU6" s="2"/>
+      <c r="AV6" s="2"/>
+      <c r="AW6" s="2"/>
+      <c r="AX6" s="2"/>
+      <c r="AY6" s="8"/>
+      <c r="AZ6" s="8"/>
+      <c r="BA6" s="8"/>
+      <c r="BB6" s="8"/>
+      <c r="BC6" s="8"/>
+      <c r="BD6" s="8"/>
+    </row>
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="24">
+        <v>0</v>
+      </c>
+      <c r="F7" s="24">
+        <v>0</v>
+      </c>
+      <c r="G7" s="24">
+        <v>0</v>
+      </c>
+      <c r="H7" s="24">
+        <v>0</v>
+      </c>
+      <c r="I7" s="24">
+        <v>0</v>
+      </c>
+      <c r="J7" s="24">
+        <v>0</v>
+      </c>
+      <c r="K7" s="24">
+        <v>0</v>
+      </c>
+      <c r="L7" s="24">
+        <v>0</v>
+      </c>
+      <c r="M7" s="24">
+        <v>0</v>
+      </c>
+      <c r="N7" s="24">
+        <v>0</v>
+      </c>
+      <c r="O7" s="24">
+        <v>0</v>
+      </c>
+      <c r="P7" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="26">
+        <v>1</v>
+      </c>
+      <c r="R7" s="24">
+        <v>0</v>
+      </c>
+      <c r="S7" s="24">
+        <v>0</v>
+      </c>
+      <c r="T7" s="24">
+        <v>0</v>
+      </c>
+      <c r="U7" s="24">
+        <v>0</v>
+      </c>
+      <c r="V7" s="24">
+        <v>0</v>
+      </c>
+      <c r="W7" s="24">
+        <v>0</v>
+      </c>
+      <c r="X7" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="24">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="24">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>3</v>
+      </c>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="2"/>
+      <c r="AM7" s="8"/>
+      <c r="AN7" s="8"/>
+      <c r="AO7" s="8"/>
+      <c r="AP7" s="8"/>
+      <c r="AQ7" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS7" s="2"/>
+      <c r="AT7" s="2"/>
+      <c r="AU7" s="2"/>
+      <c r="AV7" s="2"/>
+      <c r="AW7" s="2"/>
+      <c r="AX7" s="2"/>
+      <c r="AY7" s="8"/>
+      <c r="AZ7" s="8"/>
+      <c r="BA7" s="8"/>
+      <c r="BB7" s="8"/>
+      <c r="BC7" s="8"/>
+      <c r="BD7" s="8"/>
+    </row>
+    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
+      <c r="E8" s="24">
+        <v>0</v>
+      </c>
+      <c r="F8" s="24">
+        <v>0</v>
+      </c>
+      <c r="G8" s="24">
+        <v>0</v>
+      </c>
+      <c r="H8" s="24">
+        <v>0</v>
+      </c>
+      <c r="I8" s="24">
+        <v>0</v>
+      </c>
+      <c r="J8" s="24">
+        <v>0</v>
+      </c>
+      <c r="K8" s="24">
+        <v>0</v>
+      </c>
+      <c r="L8" s="24">
+        <v>0</v>
+      </c>
+      <c r="M8" s="24">
+        <v>0</v>
+      </c>
+      <c r="N8" s="24">
+        <v>0</v>
+      </c>
+      <c r="O8" s="24">
+        <v>0</v>
+      </c>
+      <c r="P8" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="26">
+        <v>1</v>
+      </c>
+      <c r="R8" s="24">
+        <v>0</v>
+      </c>
+      <c r="S8" s="24">
+        <v>0</v>
+      </c>
+      <c r="T8" s="24">
+        <v>0</v>
+      </c>
+      <c r="U8" s="24">
+        <v>0</v>
+      </c>
+      <c r="V8" s="24">
+        <v>0</v>
+      </c>
+      <c r="W8" s="24">
+        <v>0</v>
+      </c>
+      <c r="X8" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="24">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="24">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
+      <c r="AK8" s="2"/>
+      <c r="AL8" s="2"/>
+      <c r="AM8" s="8"/>
+      <c r="AN8" s="8"/>
+      <c r="AO8" s="8"/>
+      <c r="AP8" s="8"/>
+      <c r="AQ8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR8" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS8" s="2"/>
+      <c r="AT8" s="2"/>
+      <c r="AU8" s="2"/>
+      <c r="AV8" s="2"/>
+      <c r="AW8" s="2"/>
+      <c r="AX8" s="2"/>
+      <c r="AY8" s="8"/>
+      <c r="AZ8" s="8"/>
+      <c r="BA8" s="8"/>
+      <c r="BB8" s="8"/>
+      <c r="BC8" s="8"/>
+      <c r="BD8" s="8"/>
+    </row>
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1">
+        <v>5</v>
+      </c>
+      <c r="E9" s="22">
+        <v>0</v>
+      </c>
+      <c r="F9" s="22">
+        <v>0</v>
+      </c>
+      <c r="G9" s="22">
+        <v>0</v>
+      </c>
+      <c r="H9" s="22">
+        <v>0</v>
+      </c>
+      <c r="I9" s="22">
+        <v>0</v>
+      </c>
+      <c r="J9" s="22">
+        <v>0</v>
+      </c>
+      <c r="K9" s="22">
+        <v>0</v>
+      </c>
+      <c r="L9" s="22">
+        <v>0</v>
+      </c>
+      <c r="M9" s="22">
+        <v>0</v>
+      </c>
+      <c r="N9" s="22">
+        <v>0</v>
+      </c>
+      <c r="O9" s="22">
+        <v>0</v>
+      </c>
+      <c r="P9" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="26">
+        <v>1</v>
+      </c>
+      <c r="R9" s="22">
+        <v>0</v>
+      </c>
+      <c r="S9" s="22">
+        <v>0</v>
+      </c>
+      <c r="T9" s="22">
+        <v>0</v>
+      </c>
+      <c r="U9" s="22">
+        <v>0</v>
+      </c>
+      <c r="V9" s="22">
+        <v>0</v>
+      </c>
+      <c r="W9" s="22">
+        <v>0</v>
+      </c>
+      <c r="X9" s="22">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="22">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="22">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="22">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="1">
+        <v>5</v>
+      </c>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9"/>
+      <c r="AI9" s="9"/>
+      <c r="AJ9" s="9"/>
+      <c r="AK9" s="9"/>
+      <c r="AL9" s="9"/>
+      <c r="AM9" s="8"/>
+      <c r="AN9" s="8"/>
+      <c r="AO9" s="8"/>
+      <c r="AP9" s="8"/>
+      <c r="AQ9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR9" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS9" s="9"/>
+      <c r="AT9" s="9"/>
+      <c r="AU9" s="9"/>
+      <c r="AV9" s="9"/>
+      <c r="AW9" s="9"/>
+      <c r="AX9" s="9"/>
+      <c r="AY9" s="8"/>
+      <c r="AZ9" s="8"/>
+      <c r="BA9" s="8"/>
+      <c r="BB9" s="8"/>
+      <c r="BC9" s="8"/>
+      <c r="BD9" s="8"/>
+    </row>
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1">
+        <v>6</v>
+      </c>
+      <c r="E10" s="22">
+        <v>0</v>
+      </c>
+      <c r="F10" s="22">
+        <v>0</v>
+      </c>
+      <c r="G10" s="22">
+        <v>0</v>
+      </c>
+      <c r="H10" s="22">
+        <v>0</v>
+      </c>
+      <c r="I10" s="22">
+        <v>0</v>
+      </c>
+      <c r="J10" s="22">
+        <v>0</v>
+      </c>
+      <c r="K10" s="22">
+        <v>0</v>
+      </c>
+      <c r="L10" s="22">
+        <v>0</v>
+      </c>
+      <c r="M10" s="22">
+        <v>0</v>
+      </c>
+      <c r="N10" s="22">
+        <v>0</v>
+      </c>
+      <c r="O10" s="22">
+        <v>0</v>
+      </c>
+      <c r="P10" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="26">
+        <v>1</v>
+      </c>
+      <c r="R10" s="22">
+        <v>0</v>
+      </c>
+      <c r="S10" s="22">
+        <v>0</v>
+      </c>
+      <c r="T10" s="22">
+        <v>0</v>
+      </c>
+      <c r="U10" s="22">
+        <v>0</v>
+      </c>
+      <c r="V10" s="22">
+        <v>0</v>
+      </c>
+      <c r="W10" s="22">
+        <v>0</v>
+      </c>
+      <c r="X10" s="22">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="22">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="22">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="22">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="1">
+        <v>6</v>
+      </c>
+      <c r="AF10" s="10"/>
+      <c r="AG10" s="10"/>
+      <c r="AH10" s="10"/>
+      <c r="AI10" s="10"/>
+      <c r="AJ10" s="10"/>
+      <c r="AK10" s="10"/>
+      <c r="AL10" s="10"/>
+      <c r="AM10" s="9"/>
+      <c r="AN10" s="9"/>
+      <c r="AO10" s="9"/>
+      <c r="AP10" s="9"/>
+      <c r="AQ10" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR10" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS10" s="10"/>
+      <c r="AT10" s="10"/>
+      <c r="AU10" s="10"/>
+      <c r="AV10" s="10"/>
+      <c r="AW10" s="10"/>
+      <c r="AX10" s="10"/>
+      <c r="AY10" s="9"/>
+      <c r="AZ10" s="9"/>
+      <c r="BA10" s="9"/>
+      <c r="BB10" s="9"/>
+      <c r="BC10" s="9"/>
+      <c r="BD10" s="9"/>
+    </row>
+    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1">
+        <v>7</v>
+      </c>
+      <c r="E11" s="27">
+        <v>0</v>
+      </c>
+      <c r="F11" s="27">
+        <v>0</v>
+      </c>
+      <c r="G11" s="27">
+        <v>0</v>
+      </c>
+      <c r="H11" s="27">
+        <v>0</v>
+      </c>
+      <c r="I11" s="27">
+        <v>0</v>
+      </c>
+      <c r="J11" s="27">
+        <v>0</v>
+      </c>
+      <c r="K11" s="27">
+        <v>0</v>
+      </c>
+      <c r="L11" s="27">
+        <v>0</v>
+      </c>
+      <c r="M11" s="27">
+        <v>0</v>
+      </c>
+      <c r="N11" s="27">
+        <v>0</v>
+      </c>
+      <c r="O11" s="27">
+        <v>0</v>
+      </c>
+      <c r="P11" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="26">
+        <v>1</v>
+      </c>
+      <c r="R11" s="27">
+        <v>0</v>
+      </c>
+      <c r="S11" s="27">
+        <v>0</v>
+      </c>
+      <c r="T11" s="27">
+        <v>0</v>
+      </c>
+      <c r="U11" s="27">
+        <v>0</v>
+      </c>
+      <c r="V11" s="27">
+        <v>0</v>
+      </c>
+      <c r="W11" s="27">
+        <v>0</v>
+      </c>
+      <c r="X11" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="27">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="27">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>7</v>
+      </c>
+      <c r="AF11" s="8"/>
+      <c r="AG11" s="8"/>
+      <c r="AH11" s="8"/>
+      <c r="AI11" s="8"/>
+      <c r="AJ11" s="8"/>
+      <c r="AK11" s="8"/>
+      <c r="AL11" s="8"/>
+      <c r="AM11" s="8"/>
+      <c r="AN11" s="8"/>
+      <c r="AO11" s="8"/>
+      <c r="AP11" s="8"/>
+      <c r="AQ11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR11" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS11" s="8"/>
+      <c r="AT11" s="8"/>
+      <c r="AU11" s="8"/>
+      <c r="AV11" s="8"/>
+      <c r="AW11" s="8"/>
+      <c r="AX11" s="9"/>
+      <c r="AY11" s="8"/>
+      <c r="AZ11" s="8"/>
+      <c r="BA11" s="8"/>
+      <c r="BB11" s="8"/>
+      <c r="BC11" s="8"/>
+      <c r="BD11" s="8"/>
+    </row>
+    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1">
+        <v>8</v>
+      </c>
+      <c r="E12" s="27">
+        <v>0</v>
+      </c>
+      <c r="F12" s="27">
+        <v>0</v>
+      </c>
+      <c r="G12" s="27">
+        <v>0</v>
+      </c>
+      <c r="H12" s="27">
+        <v>0</v>
+      </c>
+      <c r="I12" s="27">
+        <v>0</v>
+      </c>
+      <c r="J12" s="27">
+        <v>0</v>
+      </c>
+      <c r="K12" s="27">
+        <v>0</v>
+      </c>
+      <c r="L12" s="27">
+        <v>0</v>
+      </c>
+      <c r="M12" s="27">
+        <v>0</v>
+      </c>
+      <c r="N12" s="27">
+        <v>0</v>
+      </c>
+      <c r="O12" s="27">
+        <v>0</v>
+      </c>
+      <c r="P12" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="26">
+        <v>1</v>
+      </c>
+      <c r="R12" s="27">
+        <v>0</v>
+      </c>
+      <c r="S12" s="27">
+        <v>0</v>
+      </c>
+      <c r="T12" s="27">
+        <v>0</v>
+      </c>
+      <c r="U12" s="27">
+        <v>0</v>
+      </c>
+      <c r="V12" s="27">
+        <v>0</v>
+      </c>
+      <c r="W12" s="27">
+        <v>0</v>
+      </c>
+      <c r="X12" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="27">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="27">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="1">
+        <v>8</v>
+      </c>
+      <c r="AF12" s="8"/>
+      <c r="AG12" s="8"/>
+      <c r="AH12" s="8"/>
+      <c r="AI12" s="8"/>
+      <c r="AJ12" s="8"/>
+      <c r="AK12" s="8"/>
+      <c r="AL12" s="8"/>
+      <c r="AM12" s="8"/>
+      <c r="AN12" s="8"/>
+      <c r="AO12" s="8"/>
+      <c r="AP12" s="8"/>
+      <c r="AQ12" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR12" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS12" s="8"/>
+      <c r="AT12" s="8"/>
+      <c r="AU12" s="8"/>
+      <c r="AV12" s="8"/>
+      <c r="AW12" s="8"/>
+      <c r="AX12" s="9"/>
+      <c r="AY12" s="8"/>
+      <c r="AZ12" s="8"/>
+      <c r="BA12" s="8"/>
+      <c r="BB12" s="8"/>
+      <c r="BC12" s="8"/>
+      <c r="BD12" s="8"/>
+    </row>
+    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1">
+        <v>9</v>
+      </c>
+      <c r="E13" s="27">
+        <v>0</v>
+      </c>
+      <c r="F13" s="27">
+        <v>0</v>
+      </c>
+      <c r="G13" s="27">
+        <v>0</v>
+      </c>
+      <c r="H13" s="27">
+        <v>0</v>
+      </c>
+      <c r="I13" s="27">
+        <v>0</v>
+      </c>
+      <c r="J13" s="27">
+        <v>0</v>
+      </c>
+      <c r="K13" s="27">
+        <v>0</v>
+      </c>
+      <c r="L13" s="27">
+        <v>0</v>
+      </c>
+      <c r="M13" s="27">
+        <v>0</v>
+      </c>
+      <c r="N13" s="27">
+        <v>0</v>
+      </c>
+      <c r="O13" s="27">
+        <v>0</v>
+      </c>
+      <c r="P13" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q13" s="26">
+        <v>1</v>
+      </c>
+      <c r="R13" s="27">
+        <v>0</v>
+      </c>
+      <c r="S13" s="27">
+        <v>0</v>
+      </c>
+      <c r="T13" s="27">
+        <v>0</v>
+      </c>
+      <c r="U13" s="27">
+        <v>0</v>
+      </c>
+      <c r="V13" s="27">
+        <v>0</v>
+      </c>
+      <c r="W13" s="27">
+        <v>0</v>
+      </c>
+      <c r="X13" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="27">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="27">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="1">
+        <v>9</v>
+      </c>
+      <c r="AF13" s="8"/>
+      <c r="AG13" s="8"/>
+      <c r="AH13" s="8"/>
+      <c r="AI13" s="8"/>
+      <c r="AJ13" s="8"/>
+      <c r="AK13" s="8"/>
+      <c r="AL13" s="8"/>
+      <c r="AM13" s="8"/>
+      <c r="AN13" s="8"/>
+      <c r="AO13" s="8"/>
+      <c r="AP13" s="8"/>
+      <c r="AQ13" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR13" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS13" s="8"/>
+      <c r="AT13" s="8"/>
+      <c r="AU13" s="8"/>
+      <c r="AV13" s="8"/>
+      <c r="AW13" s="8"/>
+      <c r="AX13" s="9"/>
+      <c r="AY13" s="8"/>
+      <c r="AZ13" s="8"/>
+      <c r="BA13" s="8"/>
+      <c r="BB13" s="8"/>
+      <c r="BC13" s="8"/>
+      <c r="BD13" s="8"/>
+    </row>
+    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="1">
+        <v>10</v>
+      </c>
+      <c r="E14" s="27">
+        <v>0</v>
+      </c>
+      <c r="F14" s="27">
+        <v>0</v>
+      </c>
+      <c r="G14" s="27">
+        <v>0</v>
+      </c>
+      <c r="H14" s="27">
+        <v>0</v>
+      </c>
+      <c r="I14" s="27">
+        <v>0</v>
+      </c>
+      <c r="J14" s="27">
+        <v>0</v>
+      </c>
+      <c r="K14" s="27">
+        <v>0</v>
+      </c>
+      <c r="L14" s="27">
+        <v>0</v>
+      </c>
+      <c r="M14" s="27">
+        <v>0</v>
+      </c>
+      <c r="N14" s="27">
+        <v>0</v>
+      </c>
+      <c r="O14" s="27">
+        <v>0</v>
+      </c>
+      <c r="P14" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="26">
+        <v>1</v>
+      </c>
+      <c r="R14" s="27">
+        <v>0</v>
+      </c>
+      <c r="S14" s="27">
+        <v>0</v>
+      </c>
+      <c r="T14" s="27">
+        <v>0</v>
+      </c>
+      <c r="U14" s="27">
+        <v>0</v>
+      </c>
+      <c r="V14" s="27">
+        <v>0</v>
+      </c>
+      <c r="W14" s="27">
+        <v>0</v>
+      </c>
+      <c r="X14" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="27">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="27">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="1">
+        <v>10</v>
+      </c>
+      <c r="AF14" s="8"/>
+      <c r="AG14" s="8"/>
+      <c r="AH14" s="8"/>
+      <c r="AI14" s="8"/>
+      <c r="AJ14" s="8"/>
+      <c r="AK14" s="8"/>
+      <c r="AL14" s="8"/>
+      <c r="AM14" s="8"/>
+      <c r="AN14" s="8"/>
+      <c r="AO14" s="8"/>
+      <c r="AP14" s="8"/>
+      <c r="AQ14" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR14" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS14" s="8"/>
+      <c r="AT14" s="8"/>
+      <c r="AU14" s="9"/>
+      <c r="AV14" s="9"/>
+      <c r="AW14" s="9"/>
+      <c r="AX14" s="9"/>
+      <c r="AY14" s="8"/>
+      <c r="AZ14" s="8"/>
+      <c r="BA14" s="8"/>
+      <c r="BB14" s="8"/>
+      <c r="BC14" s="8"/>
+      <c r="BD14" s="8"/>
+    </row>
+    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="1">
+        <v>11</v>
+      </c>
+      <c r="E15" s="28">
+        <v>4</v>
+      </c>
+      <c r="F15" s="28">
+        <v>4</v>
+      </c>
+      <c r="G15" s="28">
+        <v>4</v>
+      </c>
+      <c r="H15" s="28">
+        <v>4</v>
+      </c>
+      <c r="I15" s="28">
+        <v>4</v>
+      </c>
+      <c r="J15" s="28">
+        <v>4</v>
+      </c>
+      <c r="K15" s="28">
+        <v>4</v>
+      </c>
+      <c r="L15" s="28">
+        <v>4</v>
+      </c>
+      <c r="M15" s="28">
+        <v>4</v>
+      </c>
+      <c r="N15" s="28">
+        <v>4</v>
+      </c>
+      <c r="O15" s="28">
+        <v>4</v>
+      </c>
+      <c r="P15" s="29">
+        <v>10</v>
+      </c>
+      <c r="Q15" s="30">
+        <v>7</v>
+      </c>
+      <c r="R15" s="28">
+        <v>4</v>
+      </c>
+      <c r="S15" s="28">
+        <v>4</v>
+      </c>
+      <c r="T15" s="28">
+        <v>4</v>
+      </c>
+      <c r="U15" s="28">
+        <v>4</v>
+      </c>
+      <c r="V15" s="28">
+        <v>4</v>
+      </c>
+      <c r="W15" s="28">
+        <v>4</v>
+      </c>
+      <c r="X15" s="28">
+        <v>4</v>
+      </c>
+      <c r="Y15" s="28">
+        <v>4</v>
+      </c>
+      <c r="Z15" s="28">
+        <v>4</v>
+      </c>
+      <c r="AA15" s="28">
+        <v>4</v>
+      </c>
+      <c r="AB15" s="28">
+        <v>4</v>
+      </c>
+      <c r="AC15" s="28">
+        <v>4</v>
+      </c>
+      <c r="AE15" s="1">
+        <v>11</v>
+      </c>
+      <c r="AF15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ15" s="4"/>
+      <c r="AR15" s="3"/>
+      <c r="AS15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AV15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AW15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AX15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="BA15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="BC15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="BD15" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="1">
+        <v>12</v>
+      </c>
+      <c r="E16" s="23">
+        <v>2</v>
+      </c>
+      <c r="F16" s="23">
+        <v>2</v>
+      </c>
+      <c r="G16" s="23">
+        <v>2</v>
+      </c>
+      <c r="H16" s="23">
+        <v>2</v>
+      </c>
+      <c r="I16" s="23">
+        <v>2</v>
+      </c>
+      <c r="J16" s="23">
+        <v>2</v>
+      </c>
+      <c r="K16" s="23">
+        <v>2</v>
+      </c>
+      <c r="L16" s="23">
+        <v>2</v>
+      </c>
+      <c r="M16" s="23">
+        <v>2</v>
+      </c>
+      <c r="N16" s="23">
+        <v>2</v>
+      </c>
+      <c r="O16" s="23">
+        <v>2</v>
+      </c>
+      <c r="P16" s="30">
+        <v>8</v>
+      </c>
+      <c r="Q16" s="30">
+        <v>5</v>
+      </c>
+      <c r="R16" s="23">
+        <v>2</v>
+      </c>
+      <c r="S16" s="23">
+        <v>2</v>
+      </c>
+      <c r="T16" s="23">
+        <v>2</v>
+      </c>
+      <c r="U16" s="23">
+        <v>2</v>
+      </c>
+      <c r="V16" s="23">
+        <v>2</v>
+      </c>
+      <c r="W16" s="23">
+        <v>2</v>
+      </c>
+      <c r="X16" s="23">
+        <v>2</v>
+      </c>
+      <c r="Y16" s="23">
+        <v>2</v>
+      </c>
+      <c r="Z16" s="23">
+        <v>2</v>
+      </c>
+      <c r="AA16" s="23">
+        <v>2</v>
+      </c>
+      <c r="AB16" s="23">
+        <v>2</v>
+      </c>
+      <c r="AC16" s="23">
+        <v>2</v>
+      </c>
+      <c r="AE16" s="1">
+        <v>12</v>
+      </c>
+      <c r="AF16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="3"/>
+      <c r="AR16" s="3"/>
+      <c r="AS16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="BA16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="BB16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD16" s="18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="D17" s="1">
+        <v>13</v>
+      </c>
+      <c r="E17" s="24">
+        <v>0</v>
+      </c>
+      <c r="F17" s="24">
+        <v>0</v>
+      </c>
+      <c r="G17" s="24">
+        <v>0</v>
+      </c>
+      <c r="H17" s="24">
+        <v>0</v>
+      </c>
+      <c r="I17" s="24">
+        <v>0</v>
+      </c>
+      <c r="J17" s="24">
+        <v>0</v>
+      </c>
+      <c r="K17" s="24">
+        <v>0</v>
+      </c>
+      <c r="L17" s="24">
+        <v>0</v>
+      </c>
+      <c r="M17" s="24">
+        <v>0</v>
+      </c>
+      <c r="N17" s="24">
+        <v>0</v>
+      </c>
+      <c r="O17" s="24">
+        <v>0</v>
+      </c>
+      <c r="P17" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="31">
+        <v>1</v>
+      </c>
+      <c r="R17" s="24">
+        <v>0</v>
+      </c>
+      <c r="S17" s="24">
+        <v>0</v>
+      </c>
+      <c r="T17" s="24">
+        <v>0</v>
+      </c>
+      <c r="U17" s="24">
+        <v>0</v>
+      </c>
+      <c r="V17" s="24">
+        <v>0</v>
+      </c>
+      <c r="W17" s="24">
+        <v>0</v>
+      </c>
+      <c r="X17" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="24">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="24">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="1">
+        <v>13</v>
+      </c>
+      <c r="AF17" s="8"/>
+      <c r="AG17" s="8"/>
+      <c r="AH17" s="8"/>
+      <c r="AI17" s="8"/>
+      <c r="AJ17" s="8"/>
+      <c r="AK17" s="8"/>
+      <c r="AL17" s="8"/>
+      <c r="AM17" s="8"/>
+      <c r="AN17" s="8"/>
+      <c r="AO17" s="8"/>
+      <c r="AP17" s="8"/>
+      <c r="AQ17" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR17" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS17" s="8"/>
+      <c r="AT17" s="8"/>
+      <c r="AU17" s="9"/>
+      <c r="AV17" s="8"/>
+      <c r="AW17" s="8"/>
+      <c r="AX17" s="9"/>
+      <c r="AY17" s="8"/>
+      <c r="AZ17" s="8"/>
+      <c r="BA17" s="8"/>
+      <c r="BB17" s="8"/>
+      <c r="BC17" s="8"/>
+      <c r="BD17" s="8"/>
+    </row>
+    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="D18" s="1">
+        <v>14</v>
+      </c>
+      <c r="E18" s="24">
+        <v>0</v>
+      </c>
+      <c r="F18" s="24">
+        <v>0</v>
+      </c>
+      <c r="G18" s="24">
+        <v>0</v>
+      </c>
+      <c r="H18" s="24">
+        <v>0</v>
+      </c>
+      <c r="I18" s="24">
+        <v>0</v>
+      </c>
+      <c r="J18" s="24">
+        <v>0</v>
+      </c>
+      <c r="K18" s="24">
+        <v>0</v>
+      </c>
+      <c r="L18" s="24">
+        <v>0</v>
+      </c>
+      <c r="M18" s="24">
+        <v>0</v>
+      </c>
+      <c r="N18" s="24">
+        <v>0</v>
+      </c>
+      <c r="O18" s="24">
+        <v>0</v>
+      </c>
+      <c r="P18" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="26">
+        <v>1</v>
+      </c>
+      <c r="R18" s="24">
+        <v>0</v>
+      </c>
+      <c r="S18" s="24">
+        <v>0</v>
+      </c>
+      <c r="T18" s="24">
+        <v>0</v>
+      </c>
+      <c r="U18" s="24">
+        <v>0</v>
+      </c>
+      <c r="V18" s="24">
+        <v>0</v>
+      </c>
+      <c r="W18" s="24">
+        <v>0</v>
+      </c>
+      <c r="X18" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="24">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="24">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="1">
+        <v>14</v>
+      </c>
+      <c r="AF18" s="8"/>
+      <c r="AG18" s="8"/>
+      <c r="AH18" s="8"/>
+      <c r="AI18" s="8"/>
+      <c r="AJ18" s="8"/>
+      <c r="AK18" s="8"/>
+      <c r="AL18" s="8"/>
+      <c r="AM18" s="8"/>
+      <c r="AN18" s="8"/>
+      <c r="AO18" s="8"/>
+      <c r="AP18" s="8"/>
+      <c r="AQ18" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR18" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS18" s="8"/>
+      <c r="AT18" s="8"/>
+      <c r="AU18" s="8"/>
+      <c r="AV18" s="8"/>
+      <c r="AW18" s="8"/>
+      <c r="AX18" s="8"/>
+      <c r="AY18" s="8"/>
+      <c r="AZ18" s="8"/>
+      <c r="BA18" s="8"/>
+      <c r="BB18" s="8"/>
+      <c r="BC18" s="8"/>
+      <c r="BD18" s="8"/>
+    </row>
+    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="D19" s="1">
+        <v>15</v>
+      </c>
+      <c r="E19" s="24">
+        <v>0</v>
+      </c>
+      <c r="F19" s="24">
+        <v>0</v>
+      </c>
+      <c r="G19" s="24">
+        <v>0</v>
+      </c>
+      <c r="H19" s="24">
+        <v>0</v>
+      </c>
+      <c r="I19" s="24">
+        <v>0</v>
+      </c>
+      <c r="J19" s="24">
+        <v>0</v>
+      </c>
+      <c r="K19" s="24">
+        <v>0</v>
+      </c>
+      <c r="L19" s="24">
+        <v>0</v>
+      </c>
+      <c r="M19" s="24">
+        <v>0</v>
+      </c>
+      <c r="N19" s="24">
+        <v>0</v>
+      </c>
+      <c r="O19" s="24">
+        <v>0</v>
+      </c>
+      <c r="P19" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="26">
+        <v>1</v>
+      </c>
+      <c r="R19" s="24">
+        <v>0</v>
+      </c>
+      <c r="S19" s="24">
+        <v>0</v>
+      </c>
+      <c r="T19" s="24">
+        <v>0</v>
+      </c>
+      <c r="U19" s="24">
+        <v>0</v>
+      </c>
+      <c r="V19" s="24">
+        <v>0</v>
+      </c>
+      <c r="W19" s="24">
+        <v>0</v>
+      </c>
+      <c r="X19" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="24">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="24">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="1">
+        <v>15</v>
+      </c>
+      <c r="AF19" s="8"/>
+      <c r="AG19" s="8"/>
+      <c r="AH19" s="8"/>
+      <c r="AI19" s="8"/>
+      <c r="AJ19" s="8"/>
+      <c r="AK19" s="8"/>
+      <c r="AL19" s="8"/>
+      <c r="AM19" s="9"/>
+      <c r="AN19" s="8"/>
+      <c r="AO19" s="8"/>
+      <c r="AP19" s="8"/>
+      <c r="AQ19" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR19" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS19" s="8"/>
+      <c r="AT19" s="8"/>
+      <c r="AU19" s="2"/>
+      <c r="AV19" s="2"/>
+      <c r="AW19" s="2"/>
+      <c r="AX19" s="2"/>
+      <c r="AY19" s="2"/>
+      <c r="AZ19" s="2"/>
+      <c r="BA19" s="2"/>
+      <c r="BB19" s="2"/>
+      <c r="BC19" s="2"/>
+      <c r="BD19" s="2"/>
+    </row>
+    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="D20" s="1">
+        <v>16</v>
+      </c>
+      <c r="E20" s="24">
+        <v>0</v>
+      </c>
+      <c r="F20" s="24">
+        <v>0</v>
+      </c>
+      <c r="G20" s="24">
+        <v>0</v>
+      </c>
+      <c r="H20" s="24">
+        <v>0</v>
+      </c>
+      <c r="I20" s="24">
+        <v>0</v>
+      </c>
+      <c r="J20" s="24">
+        <v>0</v>
+      </c>
+      <c r="K20" s="24">
+        <v>0</v>
+      </c>
+      <c r="L20" s="24">
+        <v>0</v>
+      </c>
+      <c r="M20" s="24">
+        <v>0</v>
+      </c>
+      <c r="N20" s="24">
+        <v>0</v>
+      </c>
+      <c r="O20" s="24">
+        <v>0</v>
+      </c>
+      <c r="P20" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="26">
+        <v>1</v>
+      </c>
+      <c r="R20" s="24">
+        <v>0</v>
+      </c>
+      <c r="S20" s="24">
+        <v>0</v>
+      </c>
+      <c r="T20" s="24">
+        <v>0</v>
+      </c>
+      <c r="U20" s="24">
+        <v>0</v>
+      </c>
+      <c r="V20" s="24">
+        <v>0</v>
+      </c>
+      <c r="W20" s="24">
+        <v>0</v>
+      </c>
+      <c r="X20" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="24">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="24">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="1">
+        <v>16</v>
+      </c>
+      <c r="AF20" s="8"/>
+      <c r="AG20" s="8"/>
+      <c r="AH20" s="8"/>
+      <c r="AI20" s="8"/>
+      <c r="AJ20" s="8"/>
+      <c r="AK20" s="8"/>
+      <c r="AL20" s="8"/>
+      <c r="AM20" s="9"/>
+      <c r="AN20" s="8"/>
+      <c r="AO20" s="8"/>
+      <c r="AP20" s="8"/>
+      <c r="AQ20" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR20" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS20" s="8"/>
+      <c r="AT20" s="8"/>
+      <c r="AU20" s="2"/>
+      <c r="AV20" s="2"/>
+      <c r="AW20" s="2"/>
+      <c r="AX20" s="2"/>
+      <c r="AY20" s="2"/>
+      <c r="AZ20" s="2"/>
+      <c r="BA20" s="2"/>
+      <c r="BB20" s="2"/>
+      <c r="BC20" s="2"/>
+      <c r="BD20" s="2"/>
+    </row>
+    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="D21" s="1">
+        <v>17</v>
+      </c>
+      <c r="E21" s="24">
+        <v>0</v>
+      </c>
+      <c r="F21" s="24">
+        <v>0</v>
+      </c>
+      <c r="G21" s="24">
+        <v>0</v>
+      </c>
+      <c r="H21" s="24">
+        <v>0</v>
+      </c>
+      <c r="I21" s="24">
+        <v>0</v>
+      </c>
+      <c r="J21" s="24">
+        <v>0</v>
+      </c>
+      <c r="K21" s="24">
+        <v>0</v>
+      </c>
+      <c r="L21" s="24">
+        <v>0</v>
+      </c>
+      <c r="M21" s="24">
+        <v>0</v>
+      </c>
+      <c r="N21" s="24">
+        <v>0</v>
+      </c>
+      <c r="O21" s="24">
+        <v>0</v>
+      </c>
+      <c r="P21" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="26">
+        <v>1</v>
+      </c>
+      <c r="R21" s="24">
+        <v>0</v>
+      </c>
+      <c r="S21" s="24">
+        <v>0</v>
+      </c>
+      <c r="T21" s="24">
+        <v>0</v>
+      </c>
+      <c r="U21" s="24">
+        <v>0</v>
+      </c>
+      <c r="V21" s="24">
+        <v>0</v>
+      </c>
+      <c r="W21" s="24">
+        <v>0</v>
+      </c>
+      <c r="X21" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="24">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="24">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="1">
+        <v>17</v>
+      </c>
+      <c r="AF21" s="8"/>
+      <c r="AG21" s="8"/>
+      <c r="AH21" s="8"/>
+      <c r="AI21" s="8"/>
+      <c r="AJ21" s="8"/>
+      <c r="AK21" s="8"/>
+      <c r="AL21" s="8"/>
+      <c r="AM21" s="9"/>
+      <c r="AN21" s="8"/>
+      <c r="AO21" s="8"/>
+      <c r="AP21" s="8"/>
+      <c r="AQ21" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS21" s="8"/>
+      <c r="AT21" s="8"/>
+      <c r="AU21" s="2"/>
+      <c r="AV21" s="2"/>
+      <c r="AW21" s="2"/>
+      <c r="AX21" s="2"/>
+      <c r="AY21" s="2"/>
+      <c r="AZ21" s="2"/>
+      <c r="BA21" s="2"/>
+      <c r="BB21" s="2"/>
+      <c r="BC21" s="2"/>
+      <c r="BD21" s="2"/>
+    </row>
+    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="D22" s="1">
+        <v>18</v>
+      </c>
+      <c r="E22" s="22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="22">
+        <v>0</v>
+      </c>
+      <c r="G22" s="22">
+        <v>0</v>
+      </c>
+      <c r="H22" s="22">
+        <v>0</v>
+      </c>
+      <c r="I22" s="22">
+        <v>0</v>
+      </c>
+      <c r="J22" s="22">
+        <v>0</v>
+      </c>
+      <c r="K22" s="22">
+        <v>0</v>
+      </c>
+      <c r="L22" s="22">
+        <v>0</v>
+      </c>
+      <c r="M22" s="22">
+        <v>0</v>
+      </c>
+      <c r="N22" s="22">
+        <v>0</v>
+      </c>
+      <c r="O22" s="22">
+        <v>0</v>
+      </c>
+      <c r="P22" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q22" s="26">
+        <v>1</v>
+      </c>
+      <c r="R22" s="22">
+        <v>0</v>
+      </c>
+      <c r="S22" s="22">
+        <v>0</v>
+      </c>
+      <c r="T22" s="22">
+        <v>0</v>
+      </c>
+      <c r="U22" s="22">
+        <v>0</v>
+      </c>
+      <c r="V22" s="22">
+        <v>0</v>
+      </c>
+      <c r="W22" s="22">
+        <v>0</v>
+      </c>
+      <c r="X22" s="22">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="22">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="22">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="22">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="1">
+        <v>18</v>
+      </c>
+      <c r="AF22" s="9"/>
+      <c r="AG22" s="9"/>
+      <c r="AH22" s="9"/>
+      <c r="AI22" s="9"/>
+      <c r="AJ22" s="9"/>
+      <c r="AK22" s="9"/>
+      <c r="AL22" s="9"/>
+      <c r="AM22" s="9"/>
+      <c r="AN22" s="8"/>
+      <c r="AO22" s="8"/>
+      <c r="AP22" s="8"/>
+      <c r="AQ22" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR22" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS22" s="8"/>
+      <c r="AT22" s="8"/>
+      <c r="AU22" s="2"/>
+      <c r="AV22" s="2"/>
+      <c r="AW22" s="2"/>
+      <c r="AX22" s="2"/>
+      <c r="AY22" s="2"/>
+      <c r="AZ22" s="2"/>
+      <c r="BA22" s="2"/>
+      <c r="BB22" s="2"/>
+      <c r="BC22" s="2"/>
+      <c r="BD22" s="2"/>
+    </row>
+    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="D23" s="1">
+        <v>19</v>
+      </c>
+      <c r="E23" s="22">
+        <v>0</v>
+      </c>
+      <c r="F23" s="22">
+        <v>0</v>
+      </c>
+      <c r="G23" s="22">
+        <v>0</v>
+      </c>
+      <c r="H23" s="22">
+        <v>0</v>
+      </c>
+      <c r="I23" s="22">
+        <v>0</v>
+      </c>
+      <c r="J23" s="22">
+        <v>0</v>
+      </c>
+      <c r="K23" s="22">
+        <v>0</v>
+      </c>
+      <c r="L23" s="22">
+        <v>0</v>
+      </c>
+      <c r="M23" s="22">
+        <v>0</v>
+      </c>
+      <c r="N23" s="22">
+        <v>0</v>
+      </c>
+      <c r="O23" s="22">
+        <v>0</v>
+      </c>
+      <c r="P23" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q23" s="26">
+        <v>1</v>
+      </c>
+      <c r="R23" s="22">
+        <v>0</v>
+      </c>
+      <c r="S23" s="22">
+        <v>0</v>
+      </c>
+      <c r="T23" s="22">
+        <v>0</v>
+      </c>
+      <c r="U23" s="22">
+        <v>0</v>
+      </c>
+      <c r="V23" s="22">
+        <v>0</v>
+      </c>
+      <c r="W23" s="22">
+        <v>0</v>
+      </c>
+      <c r="X23" s="22">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="22">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="22">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="22">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="1">
+        <v>19</v>
+      </c>
+      <c r="AF23" s="8"/>
+      <c r="AG23" s="8"/>
+      <c r="AH23" s="8"/>
+      <c r="AI23" s="8"/>
+      <c r="AJ23" s="8"/>
+      <c r="AK23" s="8"/>
+      <c r="AL23" s="8"/>
+      <c r="AM23" s="9"/>
+      <c r="AN23" s="8"/>
+      <c r="AO23" s="8"/>
+      <c r="AP23" s="8"/>
+      <c r="AQ23" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR23" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS23" s="8"/>
+      <c r="AT23" s="8"/>
+      <c r="AU23" s="2"/>
+      <c r="AV23" s="2"/>
+      <c r="AW23" s="2"/>
+      <c r="AX23" s="2"/>
+      <c r="AY23" s="2"/>
+      <c r="AZ23" s="2"/>
+      <c r="BA23" s="2"/>
+      <c r="BB23" s="2"/>
+      <c r="BC23" s="2"/>
+      <c r="BD23" s="2"/>
+    </row>
+    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="D24" s="1">
+        <v>20</v>
+      </c>
+      <c r="E24" s="27">
+        <v>0</v>
+      </c>
+      <c r="F24" s="27">
+        <v>0</v>
+      </c>
+      <c r="G24" s="27">
+        <v>0</v>
+      </c>
+      <c r="H24" s="27">
+        <v>0</v>
+      </c>
+      <c r="I24" s="27">
+        <v>0</v>
+      </c>
+      <c r="J24" s="27">
+        <v>0</v>
+      </c>
+      <c r="K24" s="27">
+        <v>0</v>
+      </c>
+      <c r="L24" s="27">
+        <v>0</v>
+      </c>
+      <c r="M24" s="27">
+        <v>0</v>
+      </c>
+      <c r="N24" s="27">
+        <v>0</v>
+      </c>
+      <c r="O24" s="27">
+        <v>0</v>
+      </c>
+      <c r="P24" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q24" s="26">
+        <v>1</v>
+      </c>
+      <c r="R24" s="27">
+        <v>0</v>
+      </c>
+      <c r="S24" s="27">
+        <v>0</v>
+      </c>
+      <c r="T24" s="27">
+        <v>0</v>
+      </c>
+      <c r="U24" s="27">
+        <v>0</v>
+      </c>
+      <c r="V24" s="27">
+        <v>0</v>
+      </c>
+      <c r="W24" s="27">
+        <v>0</v>
+      </c>
+      <c r="X24" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="27">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="27">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE24" s="1">
+        <v>20</v>
+      </c>
+      <c r="AF24" s="8"/>
+      <c r="AG24" s="8"/>
+      <c r="AH24" s="8"/>
+      <c r="AI24" s="8"/>
+      <c r="AJ24" s="8"/>
+      <c r="AK24" s="8"/>
+      <c r="AL24" s="8"/>
+      <c r="AM24" s="9"/>
+      <c r="AN24" s="8"/>
+      <c r="AO24" s="8"/>
+      <c r="AP24" s="8"/>
+      <c r="AQ24" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR24" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS24" s="8"/>
+      <c r="AT24" s="8"/>
+      <c r="AU24" s="2"/>
+      <c r="AV24" s="2"/>
+      <c r="AW24" s="2"/>
+      <c r="AX24" s="2"/>
+      <c r="AY24" s="2"/>
+      <c r="AZ24" s="2"/>
+      <c r="BA24" s="2"/>
+      <c r="BB24" s="2"/>
+      <c r="BC24" s="2"/>
+      <c r="BD24" s="2"/>
+    </row>
+    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="D25" s="1">
+        <v>21</v>
+      </c>
+      <c r="E25" s="27">
+        <v>0</v>
+      </c>
+      <c r="F25" s="27">
+        <v>0</v>
+      </c>
+      <c r="G25" s="27">
+        <v>0</v>
+      </c>
+      <c r="H25" s="27">
+        <v>0</v>
+      </c>
+      <c r="I25" s="27">
+        <v>0</v>
+      </c>
+      <c r="J25" s="27">
+        <v>0</v>
+      </c>
+      <c r="K25" s="27">
+        <v>0</v>
+      </c>
+      <c r="L25" s="27">
+        <v>0</v>
+      </c>
+      <c r="M25" s="27">
+        <v>0</v>
+      </c>
+      <c r="N25" s="27">
+        <v>0</v>
+      </c>
+      <c r="O25" s="27">
+        <v>0</v>
+      </c>
+      <c r="P25" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q25" s="26">
+        <v>1</v>
+      </c>
+      <c r="R25" s="27">
+        <v>0</v>
+      </c>
+      <c r="S25" s="27">
+        <v>0</v>
+      </c>
+      <c r="T25" s="27">
+        <v>0</v>
+      </c>
+      <c r="U25" s="27">
+        <v>0</v>
+      </c>
+      <c r="V25" s="27">
+        <v>0</v>
+      </c>
+      <c r="W25" s="27">
+        <v>0</v>
+      </c>
+      <c r="X25" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="27">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="27">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE25" s="1">
+        <v>21</v>
+      </c>
+      <c r="AF25" s="8"/>
+      <c r="AG25" s="8"/>
+      <c r="AH25" s="8"/>
+      <c r="AI25" s="8"/>
+      <c r="AJ25" s="8"/>
+      <c r="AK25" s="8"/>
+      <c r="AL25" s="8"/>
+      <c r="AM25" s="9"/>
+      <c r="AN25" s="8"/>
+      <c r="AO25" s="8"/>
+      <c r="AP25" s="8"/>
+      <c r="AQ25" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR25" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS25" s="8"/>
+      <c r="AT25" s="8"/>
+      <c r="AU25" s="2"/>
+      <c r="AV25" s="2"/>
+      <c r="AW25" s="2"/>
+      <c r="AX25" s="2"/>
+      <c r="AY25" s="2"/>
+      <c r="AZ25" s="2"/>
+      <c r="BA25" s="2"/>
+      <c r="BB25" s="2"/>
+      <c r="BC25" s="2"/>
+      <c r="BD25" s="2"/>
+    </row>
+    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="D26" s="1">
+        <v>22</v>
+      </c>
+      <c r="E26" s="27">
+        <v>0</v>
+      </c>
+      <c r="F26" s="27">
+        <v>0</v>
+      </c>
+      <c r="G26" s="27">
+        <v>0</v>
+      </c>
+      <c r="H26" s="27">
+        <v>0</v>
+      </c>
+      <c r="I26" s="27">
+        <v>0</v>
+      </c>
+      <c r="J26" s="27">
+        <v>0</v>
+      </c>
+      <c r="K26" s="27">
+        <v>0</v>
+      </c>
+      <c r="L26" s="27">
+        <v>0</v>
+      </c>
+      <c r="M26" s="27">
+        <v>0</v>
+      </c>
+      <c r="N26" s="27">
+        <v>0</v>
+      </c>
+      <c r="O26" s="27">
+        <v>0</v>
+      </c>
+      <c r="P26" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q26" s="26">
+        <v>1</v>
+      </c>
+      <c r="R26" s="27">
+        <v>0</v>
+      </c>
+      <c r="S26" s="27">
+        <v>0</v>
+      </c>
+      <c r="T26" s="27">
+        <v>0</v>
+      </c>
+      <c r="U26" s="27">
+        <v>0</v>
+      </c>
+      <c r="V26" s="27">
+        <v>0</v>
+      </c>
+      <c r="W26" s="27">
+        <v>0</v>
+      </c>
+      <c r="X26" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="27">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="27">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="1">
+        <v>22</v>
+      </c>
+      <c r="AF26" s="8"/>
+      <c r="AG26" s="8"/>
+      <c r="AH26" s="8"/>
+      <c r="AI26" s="8"/>
+      <c r="AJ26" s="8"/>
+      <c r="AK26" s="8"/>
+      <c r="AL26" s="8"/>
+      <c r="AM26" s="9"/>
+      <c r="AN26" s="8"/>
+      <c r="AO26" s="8"/>
+      <c r="AP26" s="8"/>
+      <c r="AQ26" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR26" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS26" s="8"/>
+      <c r="AT26" s="8"/>
+      <c r="AU26" s="2"/>
+      <c r="AV26" s="2"/>
+      <c r="AW26" s="2"/>
+      <c r="AX26" s="2"/>
+      <c r="AY26" s="2"/>
+      <c r="AZ26" s="2"/>
+      <c r="BA26" s="2"/>
+      <c r="BB26" s="2"/>
+      <c r="BC26" s="2"/>
+      <c r="BD26" s="2"/>
+    </row>
+    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="D27" s="1">
+        <v>23</v>
+      </c>
+      <c r="E27" s="27">
+        <v>0</v>
+      </c>
+      <c r="F27" s="27">
+        <v>0</v>
+      </c>
+      <c r="G27" s="27">
+        <v>0</v>
+      </c>
+      <c r="H27" s="27">
+        <v>0</v>
+      </c>
+      <c r="I27" s="27">
+        <v>0</v>
+      </c>
+      <c r="J27" s="27">
+        <v>0</v>
+      </c>
+      <c r="K27" s="27">
+        <v>0</v>
+      </c>
+      <c r="L27" s="27">
+        <v>0</v>
+      </c>
+      <c r="M27" s="27">
+        <v>0</v>
+      </c>
+      <c r="N27" s="27">
+        <v>0</v>
+      </c>
+      <c r="O27" s="27">
+        <v>0</v>
+      </c>
+      <c r="P27" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q27" s="26">
+        <v>1</v>
+      </c>
+      <c r="R27" s="27">
+        <v>0</v>
+      </c>
+      <c r="S27" s="27">
+        <v>0</v>
+      </c>
+      <c r="T27" s="27">
+        <v>0</v>
+      </c>
+      <c r="U27" s="27">
+        <v>0</v>
+      </c>
+      <c r="V27" s="27">
+        <v>0</v>
+      </c>
+      <c r="W27" s="27">
+        <v>0</v>
+      </c>
+      <c r="X27" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="27">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="27">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="1">
+        <v>23</v>
+      </c>
+      <c r="AF27" s="8"/>
+      <c r="AG27" s="8"/>
+      <c r="AH27" s="8"/>
+      <c r="AI27" s="8"/>
+      <c r="AJ27" s="8"/>
+      <c r="AK27" s="8"/>
+      <c r="AL27" s="8"/>
+      <c r="AM27" s="9"/>
+      <c r="AN27" s="8"/>
+      <c r="AO27" s="8"/>
+      <c r="AP27" s="8"/>
+      <c r="AQ27" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR27" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS27" s="8"/>
+      <c r="AT27" s="8"/>
+      <c r="AU27" s="2"/>
+      <c r="AV27" s="2"/>
+      <c r="AW27" s="2"/>
+      <c r="AX27" s="2"/>
+      <c r="AY27" s="2"/>
+      <c r="AZ27" s="2"/>
+      <c r="BA27" s="2"/>
+      <c r="BB27" s="2"/>
+      <c r="BC27" s="2"/>
+      <c r="BD27" s="2"/>
+    </row>
+    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="D28" s="1">
+        <v>24</v>
+      </c>
+      <c r="E28" s="24">
+        <v>0</v>
+      </c>
+      <c r="F28" s="24">
+        <v>0</v>
+      </c>
+      <c r="G28" s="24">
+        <v>0</v>
+      </c>
+      <c r="H28" s="24">
+        <v>0</v>
+      </c>
+      <c r="I28" s="24">
+        <v>0</v>
+      </c>
+      <c r="J28" s="24">
+        <v>0</v>
+      </c>
+      <c r="K28" s="24">
+        <v>0</v>
+      </c>
+      <c r="L28" s="24">
+        <v>0</v>
+      </c>
+      <c r="M28" s="24">
+        <v>0</v>
+      </c>
+      <c r="N28" s="24">
+        <v>0</v>
+      </c>
+      <c r="O28" s="24">
+        <v>0</v>
+      </c>
+      <c r="P28" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q28" s="26">
+        <v>1</v>
+      </c>
+      <c r="R28" s="24">
+        <v>0</v>
+      </c>
+      <c r="S28" s="24">
+        <v>0</v>
+      </c>
+      <c r="T28" s="24">
+        <v>0</v>
+      </c>
+      <c r="U28" s="24">
+        <v>0</v>
+      </c>
+      <c r="V28" s="24">
+        <v>0</v>
+      </c>
+      <c r="W28" s="24">
+        <v>0</v>
+      </c>
+      <c r="X28" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="24">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="24">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="1">
+        <v>24</v>
+      </c>
+      <c r="AF28" s="2"/>
+      <c r="AG28" s="2"/>
+      <c r="AH28" s="2"/>
+      <c r="AI28" s="2"/>
+      <c r="AJ28" s="2"/>
+      <c r="AK28" s="2"/>
+      <c r="AL28" s="2"/>
+      <c r="AM28" s="9"/>
+      <c r="AN28" s="2"/>
+      <c r="AO28" s="2"/>
+      <c r="AP28" s="2"/>
+      <c r="AQ28" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR28" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS28" s="2"/>
+      <c r="AT28" s="2"/>
+      <c r="AU28" s="2"/>
+      <c r="AV28" s="2"/>
+      <c r="AW28" s="2"/>
+      <c r="AX28" s="2"/>
+      <c r="AY28" s="2"/>
+      <c r="AZ28" s="2"/>
+      <c r="BA28" s="2"/>
+      <c r="BB28" s="2"/>
+      <c r="BC28" s="2"/>
+      <c r="BD28" s="2"/>
+    </row>
+    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <v>3</v>
+      </c>
+      <c r="I29">
+        <v>4</v>
+      </c>
+      <c r="J29">
+        <v>5</v>
+      </c>
+      <c r="K29">
+        <v>6</v>
+      </c>
+      <c r="L29">
+        <v>7</v>
+      </c>
+      <c r="M29">
+        <v>8</v>
+      </c>
+      <c r="N29">
+        <v>9</v>
+      </c>
+      <c r="O29">
+        <v>10</v>
+      </c>
+      <c r="P29">
+        <v>11</v>
+      </c>
+      <c r="Q29">
+        <v>12</v>
+      </c>
+      <c r="R29">
+        <v>13</v>
+      </c>
+      <c r="S29">
+        <v>14</v>
+      </c>
+      <c r="T29">
+        <v>15</v>
+      </c>
+      <c r="U29">
+        <v>16</v>
+      </c>
+      <c r="V29">
+        <v>17</v>
+      </c>
+      <c r="W29">
+        <v>18</v>
+      </c>
+      <c r="X29">
+        <v>19</v>
+      </c>
+      <c r="Y29">
+        <v>20</v>
+      </c>
+      <c r="Z29">
+        <v>21</v>
+      </c>
+      <c r="AA29">
+        <v>21</v>
+      </c>
+      <c r="AB29">
+        <v>23</v>
+      </c>
+      <c r="AC29">
+        <v>24</v>
+      </c>
+      <c r="AF29">
+        <v>0</v>
+      </c>
+      <c r="AG29">
+        <v>1</v>
+      </c>
+      <c r="AH29">
+        <v>2</v>
+      </c>
+      <c r="AI29">
+        <v>3</v>
+      </c>
+      <c r="AJ29">
+        <v>4</v>
+      </c>
+      <c r="AK29">
+        <v>5</v>
+      </c>
+      <c r="AL29">
+        <v>6</v>
+      </c>
+      <c r="AM29">
+        <v>7</v>
+      </c>
+      <c r="AN29">
+        <v>8</v>
+      </c>
+      <c r="AO29">
+        <v>9</v>
+      </c>
+      <c r="AP29">
+        <v>10</v>
+      </c>
+      <c r="AQ29">
+        <v>11</v>
+      </c>
+      <c r="AR29">
+        <v>12</v>
+      </c>
+      <c r="AS29">
+        <v>13</v>
+      </c>
+      <c r="AT29">
+        <v>14</v>
+      </c>
+      <c r="AU29">
+        <v>15</v>
+      </c>
+      <c r="AV29">
+        <v>16</v>
+      </c>
+      <c r="AW29">
+        <v>17</v>
+      </c>
+      <c r="AX29">
+        <v>18</v>
+      </c>
+      <c r="AY29">
+        <v>19</v>
+      </c>
+      <c r="AZ29">
+        <v>20</v>
+      </c>
+      <c r="BA29">
+        <v>21</v>
+      </c>
+      <c r="BB29">
+        <v>21</v>
+      </c>
+      <c r="BC29">
+        <v>23</v>
+      </c>
+      <c r="BD29">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BI30"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:Z29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="26" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.7109375" customWidth="1"/>
+    <col min="28" max="28" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="31" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="46" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="61" width="4.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:61" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
@@ -532,7 +3964,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>0</v>
       </c>
@@ -612,7 +4044,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -648,8 +4080,83 @@
       <c r="AB4">
         <v>25</v>
       </c>
+      <c r="AK4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AN4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AO4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AP4" s="1">
+        <v>5</v>
+      </c>
+      <c r="AQ4" s="1">
+        <v>6</v>
+      </c>
+      <c r="AR4" s="1">
+        <v>7</v>
+      </c>
+      <c r="AS4" s="1">
+        <v>8</v>
+      </c>
+      <c r="AT4" s="1">
+        <v>9</v>
+      </c>
+      <c r="AU4" s="1">
+        <v>10</v>
+      </c>
+      <c r="AV4" s="1">
+        <v>11</v>
+      </c>
+      <c r="AW4" s="1">
+        <v>12</v>
+      </c>
+      <c r="AX4" s="1">
+        <v>13</v>
+      </c>
+      <c r="AY4" s="1">
+        <v>14</v>
+      </c>
+      <c r="AZ4" s="1">
+        <v>15</v>
+      </c>
+      <c r="BA4" s="1">
+        <v>16</v>
+      </c>
+      <c r="BB4" s="1">
+        <v>17</v>
+      </c>
+      <c r="BC4" s="1">
+        <v>18</v>
+      </c>
+      <c r="BD4" s="1">
+        <v>19</v>
+      </c>
+      <c r="BE4" s="1">
+        <v>20</v>
+      </c>
+      <c r="BF4" s="1">
+        <v>21</v>
+      </c>
+      <c r="BG4" s="1">
+        <v>22</v>
+      </c>
+      <c r="BH4" s="1">
+        <v>23</v>
+      </c>
+      <c r="BI4" s="1">
+        <v>24</v>
+      </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -688,8 +4195,40 @@
       <c r="AF5" t="s">
         <v>9</v>
       </c>
+      <c r="AJ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="2"/>
+      <c r="AN5" s="2"/>
+      <c r="AO5" s="2"/>
+      <c r="AP5" s="2"/>
+      <c r="AQ5" s="2"/>
+      <c r="AR5" s="8"/>
+      <c r="AS5" s="8"/>
+      <c r="AT5" s="8"/>
+      <c r="AU5" s="8"/>
+      <c r="AV5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AW5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX5" s="2"/>
+      <c r="AY5" s="2"/>
+      <c r="AZ5" s="2"/>
+      <c r="BA5" s="2"/>
+      <c r="BB5" s="2"/>
+      <c r="BC5" s="2"/>
+      <c r="BD5" s="8"/>
+      <c r="BE5" s="8"/>
+      <c r="BF5" s="8"/>
+      <c r="BG5" s="8"/>
+      <c r="BH5" s="8"/>
+      <c r="BI5" s="8"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -722,7 +4261,7 @@
       <c r="X6" s="8"/>
       <c r="Y6" s="8"/>
       <c r="Z6" s="8"/>
-      <c r="AB6" s="13">
+      <c r="AB6" s="20">
         <v>11</v>
       </c>
       <c r="AC6" s="13">
@@ -737,8 +4276,40 @@
       <c r="AF6" t="s">
         <v>10</v>
       </c>
+      <c r="AJ6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="2"/>
+      <c r="AN6" s="2"/>
+      <c r="AO6" s="2"/>
+      <c r="AP6" s="2"/>
+      <c r="AQ6" s="2"/>
+      <c r="AR6" s="8"/>
+      <c r="AS6" s="8"/>
+      <c r="AT6" s="8"/>
+      <c r="AU6" s="8"/>
+      <c r="AV6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX6" s="2"/>
+      <c r="AY6" s="2"/>
+      <c r="AZ6" s="2"/>
+      <c r="BA6" s="2"/>
+      <c r="BB6" s="2"/>
+      <c r="BC6" s="2"/>
+      <c r="BD6" s="8"/>
+      <c r="BE6" s="8"/>
+      <c r="BF6" s="8"/>
+      <c r="BG6" s="8"/>
+      <c r="BH6" s="8"/>
+      <c r="BI6" s="8"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -783,8 +4354,40 @@
       <c r="AE7" s="13">
         <v>24</v>
       </c>
+      <c r="AJ7" s="1">
+        <v>2</v>
+      </c>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="2"/>
+      <c r="AM7" s="2"/>
+      <c r="AN7" s="2"/>
+      <c r="AO7" s="2"/>
+      <c r="AP7" s="2"/>
+      <c r="AQ7" s="2"/>
+      <c r="AR7" s="8"/>
+      <c r="AS7" s="8"/>
+      <c r="AT7" s="8"/>
+      <c r="AU7" s="8"/>
+      <c r="AV7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX7" s="2"/>
+      <c r="AY7" s="2"/>
+      <c r="AZ7" s="2"/>
+      <c r="BA7" s="2"/>
+      <c r="BB7" s="2"/>
+      <c r="BC7" s="2"/>
+      <c r="BD7" s="8"/>
+      <c r="BE7" s="8"/>
+      <c r="BF7" s="8"/>
+      <c r="BG7" s="8"/>
+      <c r="BH7" s="8"/>
+      <c r="BI7" s="8"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -829,8 +4432,40 @@
       <c r="AE8" s="15">
         <v>12</v>
       </c>
+      <c r="AJ8" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK8" s="2"/>
+      <c r="AL8" s="2"/>
+      <c r="AM8" s="2"/>
+      <c r="AN8" s="2"/>
+      <c r="AO8" s="2"/>
+      <c r="AP8" s="2"/>
+      <c r="AQ8" s="2"/>
+      <c r="AR8" s="8"/>
+      <c r="AS8" s="8"/>
+      <c r="AT8" s="8"/>
+      <c r="AU8" s="8"/>
+      <c r="AV8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW8" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX8" s="2"/>
+      <c r="AY8" s="2"/>
+      <c r="AZ8" s="2"/>
+      <c r="BA8" s="2"/>
+      <c r="BB8" s="2"/>
+      <c r="BC8" s="2"/>
+      <c r="BD8" s="8"/>
+      <c r="BE8" s="8"/>
+      <c r="BF8" s="8"/>
+      <c r="BG8" s="8"/>
+      <c r="BH8" s="8"/>
+      <c r="BI8" s="8"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -875,8 +4510,40 @@
       <c r="AE9" s="15">
         <v>0</v>
       </c>
+      <c r="AJ9" s="1">
+        <v>4</v>
+      </c>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="2"/>
+      <c r="AN9" s="2"/>
+      <c r="AO9" s="2"/>
+      <c r="AP9" s="2"/>
+      <c r="AQ9" s="2"/>
+      <c r="AR9" s="8"/>
+      <c r="AS9" s="8"/>
+      <c r="AT9" s="8"/>
+      <c r="AU9" s="8"/>
+      <c r="AV9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW9" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX9" s="2"/>
+      <c r="AY9" s="2"/>
+      <c r="AZ9" s="2"/>
+      <c r="BA9" s="2"/>
+      <c r="BB9" s="2"/>
+      <c r="BC9" s="2"/>
+      <c r="BD9" s="8"/>
+      <c r="BE9" s="8"/>
+      <c r="BF9" s="8"/>
+      <c r="BG9" s="8"/>
+      <c r="BH9" s="8"/>
+      <c r="BI9" s="8"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -921,8 +4588,40 @@
       <c r="AE10" s="19">
         <v>12</v>
       </c>
+      <c r="AJ10" s="1">
+        <v>5</v>
+      </c>
+      <c r="AK10" s="9"/>
+      <c r="AL10" s="9"/>
+      <c r="AM10" s="9"/>
+      <c r="AN10" s="9"/>
+      <c r="AO10" s="9"/>
+      <c r="AP10" s="9"/>
+      <c r="AQ10" s="9"/>
+      <c r="AR10" s="8"/>
+      <c r="AS10" s="8"/>
+      <c r="AT10" s="8"/>
+      <c r="AU10" s="8"/>
+      <c r="AV10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW10" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX10" s="9"/>
+      <c r="AY10" s="9"/>
+      <c r="AZ10" s="9"/>
+      <c r="BA10" s="9"/>
+      <c r="BB10" s="9"/>
+      <c r="BC10" s="9"/>
+      <c r="BD10" s="8"/>
+      <c r="BE10" s="8"/>
+      <c r="BF10" s="8"/>
+      <c r="BG10" s="8"/>
+      <c r="BH10" s="8"/>
+      <c r="BI10" s="8"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -967,8 +4666,40 @@
       <c r="AE11" s="19">
         <v>12</v>
       </c>
+      <c r="AJ11" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK11" s="10"/>
+      <c r="AL11" s="10"/>
+      <c r="AM11" s="10"/>
+      <c r="AN11" s="10"/>
+      <c r="AO11" s="10"/>
+      <c r="AP11" s="10"/>
+      <c r="AQ11" s="10"/>
+      <c r="AR11" s="9"/>
+      <c r="AS11" s="9"/>
+      <c r="AT11" s="9"/>
+      <c r="AU11" s="9"/>
+      <c r="AV11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW11" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX11" s="10"/>
+      <c r="AY11" s="10"/>
+      <c r="AZ11" s="10"/>
+      <c r="BA11" s="10"/>
+      <c r="BB11" s="10"/>
+      <c r="BC11" s="10"/>
+      <c r="BD11" s="9"/>
+      <c r="BE11" s="9"/>
+      <c r="BF11" s="9"/>
+      <c r="BG11" s="9"/>
+      <c r="BH11" s="9"/>
+      <c r="BI11" s="9"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -1013,8 +4744,40 @@
       <c r="AE12" s="17">
         <v>11</v>
       </c>
+      <c r="AJ12" s="1">
+        <v>7</v>
+      </c>
+      <c r="AK12" s="8"/>
+      <c r="AL12" s="8"/>
+      <c r="AM12" s="8"/>
+      <c r="AN12" s="8"/>
+      <c r="AO12" s="8"/>
+      <c r="AP12" s="8"/>
+      <c r="AQ12" s="8"/>
+      <c r="AR12" s="8"/>
+      <c r="AS12" s="8"/>
+      <c r="AT12" s="8"/>
+      <c r="AU12" s="8"/>
+      <c r="AV12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW12" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX12" s="8"/>
+      <c r="AY12" s="8"/>
+      <c r="AZ12" s="8"/>
+      <c r="BA12" s="8"/>
+      <c r="BB12" s="8"/>
+      <c r="BC12" s="9"/>
+      <c r="BD12" s="8"/>
+      <c r="BE12" s="8"/>
+      <c r="BF12" s="8"/>
+      <c r="BG12" s="8"/>
+      <c r="BH12" s="8"/>
+      <c r="BI12" s="8"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -1059,8 +4822,40 @@
       <c r="AE13" s="17">
         <v>11</v>
       </c>
+      <c r="AJ13" s="1">
+        <v>8</v>
+      </c>
+      <c r="AK13" s="8"/>
+      <c r="AL13" s="8"/>
+      <c r="AM13" s="8"/>
+      <c r="AN13" s="8"/>
+      <c r="AO13" s="8"/>
+      <c r="AP13" s="8"/>
+      <c r="AQ13" s="8"/>
+      <c r="AR13" s="8"/>
+      <c r="AS13" s="8"/>
+      <c r="AT13" s="8"/>
+      <c r="AU13" s="8"/>
+      <c r="AV13" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW13" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX13" s="8"/>
+      <c r="AY13" s="8"/>
+      <c r="AZ13" s="8"/>
+      <c r="BA13" s="8"/>
+      <c r="BB13" s="8"/>
+      <c r="BC13" s="9"/>
+      <c r="BD13" s="8"/>
+      <c r="BE13" s="8"/>
+      <c r="BF13" s="8"/>
+      <c r="BG13" s="8"/>
+      <c r="BH13" s="8"/>
+      <c r="BI13" s="8"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -1097,8 +4892,40 @@
       <c r="AC14" s="11"/>
       <c r="AD14" s="11"/>
       <c r="AE14" s="11"/>
+      <c r="AJ14" s="1">
+        <v>9</v>
+      </c>
+      <c r="AK14" s="8"/>
+      <c r="AL14" s="8"/>
+      <c r="AM14" s="8"/>
+      <c r="AN14" s="8"/>
+      <c r="AO14" s="8"/>
+      <c r="AP14" s="8"/>
+      <c r="AQ14" s="8"/>
+      <c r="AR14" s="8"/>
+      <c r="AS14" s="8"/>
+      <c r="AT14" s="8"/>
+      <c r="AU14" s="8"/>
+      <c r="AV14" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW14" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX14" s="8"/>
+      <c r="AY14" s="8"/>
+      <c r="AZ14" s="8"/>
+      <c r="BA14" s="8"/>
+      <c r="BB14" s="8"/>
+      <c r="BC14" s="9"/>
+      <c r="BD14" s="8"/>
+      <c r="BE14" s="8"/>
+      <c r="BF14" s="8"/>
+      <c r="BG14" s="8"/>
+      <c r="BH14" s="8"/>
+      <c r="BI14" s="8"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -1177,8 +5004,40 @@
       <c r="AC15" s="11"/>
       <c r="AD15" s="11"/>
       <c r="AE15" s="11"/>
+      <c r="AJ15" s="1">
+        <v>10</v>
+      </c>
+      <c r="AK15" s="8"/>
+      <c r="AL15" s="8"/>
+      <c r="AM15" s="8"/>
+      <c r="AN15" s="8"/>
+      <c r="AO15" s="8"/>
+      <c r="AP15" s="8"/>
+      <c r="AQ15" s="8"/>
+      <c r="AR15" s="8"/>
+      <c r="AS15" s="8"/>
+      <c r="AT15" s="8"/>
+      <c r="AU15" s="8"/>
+      <c r="AV15" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW15" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX15" s="8"/>
+      <c r="AY15" s="8"/>
+      <c r="AZ15" s="9"/>
+      <c r="BA15" s="9"/>
+      <c r="BB15" s="9"/>
+      <c r="BC15" s="9"/>
+      <c r="BD15" s="8"/>
+      <c r="BE15" s="8"/>
+      <c r="BF15" s="8"/>
+      <c r="BG15" s="8"/>
+      <c r="BH15" s="8"/>
+      <c r="BI15" s="8"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -1257,8 +5116,84 @@
       <c r="AC16" s="11"/>
       <c r="AD16" s="11"/>
       <c r="AE16" s="11"/>
+      <c r="AJ16" s="1">
+        <v>11</v>
+      </c>
+      <c r="AK16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AR16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AV16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AW16" s="3"/>
+      <c r="AX16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="BA16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="BC16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="BD16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="BE16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="BF16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="BG16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="BH16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI16" s="16" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -1295,8 +5230,84 @@
       <c r="AC17" s="11"/>
       <c r="AD17" s="11"/>
       <c r="AE17" s="11"/>
+      <c r="AJ17" s="1">
+        <v>12</v>
+      </c>
+      <c r="AK17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AW17" s="3"/>
+      <c r="AX17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="BA17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="BB17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="BE17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="BF17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="BI17" s="18" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -1333,8 +5344,40 @@
       <c r="AC18" s="11"/>
       <c r="AD18" s="11"/>
       <c r="AE18" s="11"/>
+      <c r="AJ18" s="1">
+        <v>13</v>
+      </c>
+      <c r="AK18" s="8"/>
+      <c r="AL18" s="8"/>
+      <c r="AM18" s="8"/>
+      <c r="AN18" s="8"/>
+      <c r="AO18" s="8"/>
+      <c r="AP18" s="8"/>
+      <c r="AQ18" s="8"/>
+      <c r="AR18" s="8"/>
+      <c r="AS18" s="8"/>
+      <c r="AT18" s="8"/>
+      <c r="AU18" s="8"/>
+      <c r="AV18" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW18" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX18" s="8"/>
+      <c r="AY18" s="8"/>
+      <c r="AZ18" s="9"/>
+      <c r="BA18" s="8"/>
+      <c r="BB18" s="8"/>
+      <c r="BC18" s="9"/>
+      <c r="BD18" s="8"/>
+      <c r="BE18" s="8"/>
+      <c r="BF18" s="8"/>
+      <c r="BG18" s="8"/>
+      <c r="BH18" s="8"/>
+      <c r="BI18" s="8"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -1371,8 +5414,40 @@
       <c r="AC19" s="11"/>
       <c r="AD19" s="11"/>
       <c r="AE19" s="11"/>
+      <c r="AJ19" s="1">
+        <v>14</v>
+      </c>
+      <c r="AK19" s="8"/>
+      <c r="AL19" s="8"/>
+      <c r="AM19" s="8"/>
+      <c r="AN19" s="8"/>
+      <c r="AO19" s="8"/>
+      <c r="AP19" s="8"/>
+      <c r="AQ19" s="8"/>
+      <c r="AR19" s="8"/>
+      <c r="AS19" s="8"/>
+      <c r="AT19" s="8"/>
+      <c r="AU19" s="8"/>
+      <c r="AV19" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW19" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX19" s="8"/>
+      <c r="AY19" s="8"/>
+      <c r="AZ19" s="8"/>
+      <c r="BA19" s="8"/>
+      <c r="BB19" s="8"/>
+      <c r="BC19" s="8"/>
+      <c r="BD19" s="8"/>
+      <c r="BE19" s="8"/>
+      <c r="BF19" s="8"/>
+      <c r="BG19" s="8"/>
+      <c r="BH19" s="8"/>
+      <c r="BI19" s="8"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -1409,8 +5484,40 @@
       <c r="AC20" s="11"/>
       <c r="AD20" s="11"/>
       <c r="AE20" s="11"/>
+      <c r="AJ20" s="1">
+        <v>15</v>
+      </c>
+      <c r="AK20" s="8"/>
+      <c r="AL20" s="8"/>
+      <c r="AM20" s="8"/>
+      <c r="AN20" s="8"/>
+      <c r="AO20" s="8"/>
+      <c r="AP20" s="8"/>
+      <c r="AQ20" s="8"/>
+      <c r="AR20" s="9"/>
+      <c r="AS20" s="8"/>
+      <c r="AT20" s="8"/>
+      <c r="AU20" s="8"/>
+      <c r="AV20" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW20" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX20" s="8"/>
+      <c r="AY20" s="8"/>
+      <c r="AZ20" s="2"/>
+      <c r="BA20" s="2"/>
+      <c r="BB20" s="2"/>
+      <c r="BC20" s="2"/>
+      <c r="BD20" s="2"/>
+      <c r="BE20" s="2"/>
+      <c r="BF20" s="2"/>
+      <c r="BG20" s="2"/>
+      <c r="BH20" s="2"/>
+      <c r="BI20" s="2"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -1447,8 +5554,40 @@
       <c r="AC21" s="11"/>
       <c r="AD21" s="11"/>
       <c r="AE21" s="11"/>
+      <c r="AJ21" s="1">
+        <v>16</v>
+      </c>
+      <c r="AK21" s="8"/>
+      <c r="AL21" s="8"/>
+      <c r="AM21" s="8"/>
+      <c r="AN21" s="8"/>
+      <c r="AO21" s="8"/>
+      <c r="AP21" s="8"/>
+      <c r="AQ21" s="8"/>
+      <c r="AR21" s="9"/>
+      <c r="AS21" s="8"/>
+      <c r="AT21" s="8"/>
+      <c r="AU21" s="8"/>
+      <c r="AV21" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX21" s="8"/>
+      <c r="AY21" s="8"/>
+      <c r="AZ21" s="2"/>
+      <c r="BA21" s="2"/>
+      <c r="BB21" s="2"/>
+      <c r="BC21" s="2"/>
+      <c r="BD21" s="2"/>
+      <c r="BE21" s="2"/>
+      <c r="BF21" s="2"/>
+      <c r="BG21" s="2"/>
+      <c r="BH21" s="2"/>
+      <c r="BI21" s="2"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -1485,8 +5624,40 @@
       <c r="AC22" s="11"/>
       <c r="AD22" s="11"/>
       <c r="AE22" s="11"/>
+      <c r="AJ22" s="1">
+        <v>17</v>
+      </c>
+      <c r="AK22" s="8"/>
+      <c r="AL22" s="8"/>
+      <c r="AM22" s="8"/>
+      <c r="AN22" s="8"/>
+      <c r="AO22" s="8"/>
+      <c r="AP22" s="8"/>
+      <c r="AQ22" s="8"/>
+      <c r="AR22" s="9"/>
+      <c r="AS22" s="8"/>
+      <c r="AT22" s="8"/>
+      <c r="AU22" s="8"/>
+      <c r="AV22" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW22" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX22" s="8"/>
+      <c r="AY22" s="8"/>
+      <c r="AZ22" s="2"/>
+      <c r="BA22" s="2"/>
+      <c r="BB22" s="2"/>
+      <c r="BC22" s="2"/>
+      <c r="BD22" s="2"/>
+      <c r="BE22" s="2"/>
+      <c r="BF22" s="2"/>
+      <c r="BG22" s="2"/>
+      <c r="BH22" s="2"/>
+      <c r="BI22" s="2"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -1519,8 +5690,40 @@
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
+      <c r="AJ23" s="1">
+        <v>18</v>
+      </c>
+      <c r="AK23" s="9"/>
+      <c r="AL23" s="9"/>
+      <c r="AM23" s="9"/>
+      <c r="AN23" s="9"/>
+      <c r="AO23" s="9"/>
+      <c r="AP23" s="9"/>
+      <c r="AQ23" s="9"/>
+      <c r="AR23" s="9"/>
+      <c r="AS23" s="8"/>
+      <c r="AT23" s="8"/>
+      <c r="AU23" s="8"/>
+      <c r="AV23" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW23" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX23" s="8"/>
+      <c r="AY23" s="8"/>
+      <c r="AZ23" s="2"/>
+      <c r="BA23" s="2"/>
+      <c r="BB23" s="2"/>
+      <c r="BC23" s="2"/>
+      <c r="BD23" s="2"/>
+      <c r="BE23" s="2"/>
+      <c r="BF23" s="2"/>
+      <c r="BG23" s="2"/>
+      <c r="BH23" s="2"/>
+      <c r="BI23" s="2"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -1553,8 +5756,40 @@
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
+      <c r="AJ24" s="1">
+        <v>19</v>
+      </c>
+      <c r="AK24" s="8"/>
+      <c r="AL24" s="8"/>
+      <c r="AM24" s="8"/>
+      <c r="AN24" s="8"/>
+      <c r="AO24" s="8"/>
+      <c r="AP24" s="8"/>
+      <c r="AQ24" s="8"/>
+      <c r="AR24" s="9"/>
+      <c r="AS24" s="8"/>
+      <c r="AT24" s="8"/>
+      <c r="AU24" s="8"/>
+      <c r="AV24" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW24" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX24" s="8"/>
+      <c r="AY24" s="8"/>
+      <c r="AZ24" s="2"/>
+      <c r="BA24" s="2"/>
+      <c r="BB24" s="2"/>
+      <c r="BC24" s="2"/>
+      <c r="BD24" s="2"/>
+      <c r="BE24" s="2"/>
+      <c r="BF24" s="2"/>
+      <c r="BG24" s="2"/>
+      <c r="BH24" s="2"/>
+      <c r="BI24" s="2"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -1587,8 +5822,40 @@
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
+      <c r="AJ25" s="1">
+        <v>20</v>
+      </c>
+      <c r="AK25" s="8"/>
+      <c r="AL25" s="8"/>
+      <c r="AM25" s="8"/>
+      <c r="AN25" s="8"/>
+      <c r="AO25" s="8"/>
+      <c r="AP25" s="8"/>
+      <c r="AQ25" s="8"/>
+      <c r="AR25" s="9"/>
+      <c r="AS25" s="8"/>
+      <c r="AT25" s="8"/>
+      <c r="AU25" s="8"/>
+      <c r="AV25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW25" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX25" s="8"/>
+      <c r="AY25" s="8"/>
+      <c r="AZ25" s="2"/>
+      <c r="BA25" s="2"/>
+      <c r="BB25" s="2"/>
+      <c r="BC25" s="2"/>
+      <c r="BD25" s="2"/>
+      <c r="BE25" s="2"/>
+      <c r="BF25" s="2"/>
+      <c r="BG25" s="2"/>
+      <c r="BH25" s="2"/>
+      <c r="BI25" s="2"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -1621,8 +5888,40 @@
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
+      <c r="AJ26" s="1">
+        <v>21</v>
+      </c>
+      <c r="AK26" s="8"/>
+      <c r="AL26" s="8"/>
+      <c r="AM26" s="8"/>
+      <c r="AN26" s="8"/>
+      <c r="AO26" s="8"/>
+      <c r="AP26" s="8"/>
+      <c r="AQ26" s="8"/>
+      <c r="AR26" s="9"/>
+      <c r="AS26" s="8"/>
+      <c r="AT26" s="8"/>
+      <c r="AU26" s="8"/>
+      <c r="AV26" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW26" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX26" s="8"/>
+      <c r="AY26" s="8"/>
+      <c r="AZ26" s="2"/>
+      <c r="BA26" s="2"/>
+      <c r="BB26" s="2"/>
+      <c r="BC26" s="2"/>
+      <c r="BD26" s="2"/>
+      <c r="BE26" s="2"/>
+      <c r="BF26" s="2"/>
+      <c r="BG26" s="2"/>
+      <c r="BH26" s="2"/>
+      <c r="BI26" s="2"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -1655,8 +5954,40 @@
       <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
+      <c r="AJ27" s="1">
+        <v>22</v>
+      </c>
+      <c r="AK27" s="8"/>
+      <c r="AL27" s="8"/>
+      <c r="AM27" s="8"/>
+      <c r="AN27" s="8"/>
+      <c r="AO27" s="8"/>
+      <c r="AP27" s="8"/>
+      <c r="AQ27" s="8"/>
+      <c r="AR27" s="9"/>
+      <c r="AS27" s="8"/>
+      <c r="AT27" s="8"/>
+      <c r="AU27" s="8"/>
+      <c r="AV27" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW27" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX27" s="8"/>
+      <c r="AY27" s="8"/>
+      <c r="AZ27" s="2"/>
+      <c r="BA27" s="2"/>
+      <c r="BB27" s="2"/>
+      <c r="BC27" s="2"/>
+      <c r="BD27" s="2"/>
+      <c r="BE27" s="2"/>
+      <c r="BF27" s="2"/>
+      <c r="BG27" s="2"/>
+      <c r="BH27" s="2"/>
+      <c r="BI27" s="2"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -1689,8 +6020,40 @@
       <c r="X28" s="2"/>
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
+      <c r="AJ28" s="1">
+        <v>23</v>
+      </c>
+      <c r="AK28" s="8"/>
+      <c r="AL28" s="8"/>
+      <c r="AM28" s="8"/>
+      <c r="AN28" s="8"/>
+      <c r="AO28" s="8"/>
+      <c r="AP28" s="8"/>
+      <c r="AQ28" s="8"/>
+      <c r="AR28" s="9"/>
+      <c r="AS28" s="8"/>
+      <c r="AT28" s="8"/>
+      <c r="AU28" s="8"/>
+      <c r="AV28" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW28" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX28" s="8"/>
+      <c r="AY28" s="8"/>
+      <c r="AZ28" s="2"/>
+      <c r="BA28" s="2"/>
+      <c r="BB28" s="2"/>
+      <c r="BC28" s="2"/>
+      <c r="BD28" s="2"/>
+      <c r="BE28" s="2"/>
+      <c r="BF28" s="2"/>
+      <c r="BG28" s="2"/>
+      <c r="BH28" s="2"/>
+      <c r="BI28" s="2"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:61" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>0</v>
       </c>
@@ -1764,6 +6127,115 @@
         <v>23</v>
       </c>
       <c r="Z29">
+        <v>24</v>
+      </c>
+      <c r="AJ29" s="1">
+        <v>24</v>
+      </c>
+      <c r="AK29" s="2"/>
+      <c r="AL29" s="2"/>
+      <c r="AM29" s="2"/>
+      <c r="AN29" s="2"/>
+      <c r="AO29" s="2"/>
+      <c r="AP29" s="2"/>
+      <c r="AQ29" s="2"/>
+      <c r="AR29" s="9"/>
+      <c r="AS29" s="2"/>
+      <c r="AT29" s="2"/>
+      <c r="AU29" s="2"/>
+      <c r="AV29" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AW29" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX29" s="2"/>
+      <c r="AY29" s="2"/>
+      <c r="AZ29" s="2"/>
+      <c r="BA29" s="2"/>
+      <c r="BB29" s="2"/>
+      <c r="BC29" s="2"/>
+      <c r="BD29" s="2"/>
+      <c r="BE29" s="2"/>
+      <c r="BF29" s="2"/>
+      <c r="BG29" s="2"/>
+      <c r="BH29" s="2"/>
+      <c r="BI29" s="2"/>
+    </row>
+    <row r="30" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="AK30">
+        <v>0</v>
+      </c>
+      <c r="AL30">
+        <v>1</v>
+      </c>
+      <c r="AM30">
+        <v>2</v>
+      </c>
+      <c r="AN30">
+        <v>3</v>
+      </c>
+      <c r="AO30">
+        <v>4</v>
+      </c>
+      <c r="AP30">
+        <v>5</v>
+      </c>
+      <c r="AQ30">
+        <v>6</v>
+      </c>
+      <c r="AR30">
+        <v>7</v>
+      </c>
+      <c r="AS30">
+        <v>8</v>
+      </c>
+      <c r="AT30">
+        <v>9</v>
+      </c>
+      <c r="AU30">
+        <v>10</v>
+      </c>
+      <c r="AV30">
+        <v>11</v>
+      </c>
+      <c r="AW30">
+        <v>12</v>
+      </c>
+      <c r="AX30">
+        <v>13</v>
+      </c>
+      <c r="AY30">
+        <v>14</v>
+      </c>
+      <c r="AZ30">
+        <v>15</v>
+      </c>
+      <c r="BA30">
+        <v>16</v>
+      </c>
+      <c r="BB30">
+        <v>17</v>
+      </c>
+      <c r="BC30">
+        <v>18</v>
+      </c>
+      <c r="BD30">
+        <v>19</v>
+      </c>
+      <c r="BE30">
+        <v>20</v>
+      </c>
+      <c r="BF30">
+        <v>21</v>
+      </c>
+      <c r="BG30">
+        <v>21</v>
+      </c>
+      <c r="BH30">
+        <v>23</v>
+      </c>
+      <c r="BI30">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implementação do novo leitor de malha
</commit_message>
<xml_diff>
--- a/malhas/malhas-mao-dupla.xlsx
+++ b/malhas/malhas-mao-dupla.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
-    <sheet name="malha-exemplo1" sheetId="1" r:id="rId2"/>
+    <sheet name="Planilha2" sheetId="3" r:id="rId2"/>
+    <sheet name="malha-exemplo1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="29">
   <si>
     <t>→</t>
   </si>
@@ -226,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -286,6 +287,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -600,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3917,10 +3927,688 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="4" max="7" width="3.42578125" customWidth="1"/>
+    <col min="8" max="8" width="3" customWidth="1"/>
+    <col min="9" max="12" width="3.42578125" customWidth="1"/>
+    <col min="13" max="13" width="2.5703125" customWidth="1"/>
+    <col min="14" max="14" width="3.140625" customWidth="1"/>
+    <col min="15" max="15" width="3.28515625" customWidth="1"/>
+    <col min="16" max="16" width="3.42578125" customWidth="1"/>
+    <col min="17" max="17" width="3.85546875" customWidth="1"/>
+    <col min="18" max="19" width="3.28515625" customWidth="1"/>
+    <col min="20" max="20" width="3.5703125" customWidth="1"/>
+    <col min="21" max="21" width="4.140625" customWidth="1"/>
+    <col min="22" max="22" width="4.28515625" customWidth="1"/>
+    <col min="23" max="29" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="41" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="56" width="5.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="33"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33">
+        <v>0</v>
+      </c>
+      <c r="F4" s="33">
+        <v>1</v>
+      </c>
+      <c r="G4" s="33">
+        <v>2</v>
+      </c>
+      <c r="H4" s="33">
+        <v>3</v>
+      </c>
+      <c r="I4" s="33">
+        <v>4</v>
+      </c>
+      <c r="J4" s="33">
+        <v>5</v>
+      </c>
+      <c r="K4" s="33">
+        <v>6</v>
+      </c>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33">
+        <v>0</v>
+      </c>
+      <c r="O4" s="33">
+        <v>1</v>
+      </c>
+      <c r="P4" s="33">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="33">
+        <v>3</v>
+      </c>
+      <c r="R4" s="33">
+        <v>4</v>
+      </c>
+      <c r="S4" s="33">
+        <v>5</v>
+      </c>
+      <c r="T4" s="33">
+        <v>6</v>
+      </c>
+      <c r="U4" s="33">
+        <v>7</v>
+      </c>
+      <c r="V4" s="33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="33">
+        <v>0</v>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33">
+        <v>0</v>
+      </c>
+      <c r="N5" s="24">
+        <v>0</v>
+      </c>
+      <c r="O5" s="24">
+        <v>0</v>
+      </c>
+      <c r="P5" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="34">
+        <v>1</v>
+      </c>
+      <c r="R5" s="24">
+        <v>0</v>
+      </c>
+      <c r="S5" s="24">
+        <v>0</v>
+      </c>
+      <c r="T5" s="24">
+        <v>0</v>
+      </c>
+      <c r="U5" s="24">
+        <v>0</v>
+      </c>
+      <c r="V5" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="33">
+        <v>1</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="24"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33">
+        <v>1</v>
+      </c>
+      <c r="N6" s="24">
+        <v>0</v>
+      </c>
+      <c r="O6" s="24">
+        <v>0</v>
+      </c>
+      <c r="P6" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="34">
+        <v>1</v>
+      </c>
+      <c r="R6" s="24">
+        <v>0</v>
+      </c>
+      <c r="S6" s="24">
+        <v>0</v>
+      </c>
+      <c r="T6" s="24">
+        <v>0</v>
+      </c>
+      <c r="U6" s="24">
+        <v>0</v>
+      </c>
+      <c r="V6" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="33">
+        <v>2</v>
+      </c>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33">
+        <v>2</v>
+      </c>
+      <c r="N7" s="24">
+        <v>0</v>
+      </c>
+      <c r="O7" s="24">
+        <v>0</v>
+      </c>
+      <c r="P7" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="34">
+        <v>1</v>
+      </c>
+      <c r="R7" s="24">
+        <v>0</v>
+      </c>
+      <c r="S7" s="24">
+        <v>0</v>
+      </c>
+      <c r="T7" s="24">
+        <v>0</v>
+      </c>
+      <c r="U7" s="24">
+        <v>0</v>
+      </c>
+      <c r="V7" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="33">
+        <v>3</v>
+      </c>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33">
+        <v>3</v>
+      </c>
+      <c r="N8" s="24">
+        <v>0</v>
+      </c>
+      <c r="O8" s="24">
+        <v>0</v>
+      </c>
+      <c r="P8" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="34">
+        <v>1</v>
+      </c>
+      <c r="R8" s="24">
+        <v>0</v>
+      </c>
+      <c r="S8" s="24">
+        <v>0</v>
+      </c>
+      <c r="T8" s="24">
+        <v>0</v>
+      </c>
+      <c r="U8" s="24">
+        <v>0</v>
+      </c>
+      <c r="V8" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="33">
+        <v>4</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="24"/>
+      <c r="I9" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33">
+        <v>4</v>
+      </c>
+      <c r="N9" s="34">
+        <v>4</v>
+      </c>
+      <c r="O9" s="34">
+        <v>4</v>
+      </c>
+      <c r="P9" s="34">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="24">
+        <v>13</v>
+      </c>
+      <c r="R9" s="34">
+        <v>4</v>
+      </c>
+      <c r="S9" s="34">
+        <v>4</v>
+      </c>
+      <c r="T9" s="34">
+        <v>4</v>
+      </c>
+      <c r="U9" s="24">
+        <v>4</v>
+      </c>
+      <c r="V9" s="27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="33">
+        <v>5</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33">
+        <v>5</v>
+      </c>
+      <c r="N10" s="24">
+        <v>0</v>
+      </c>
+      <c r="O10" s="24">
+        <v>0</v>
+      </c>
+      <c r="P10" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="34">
+        <v>3</v>
+      </c>
+      <c r="R10" s="24">
+        <v>0</v>
+      </c>
+      <c r="S10" s="24">
+        <v>0</v>
+      </c>
+      <c r="T10" s="24">
+        <v>0</v>
+      </c>
+      <c r="U10" s="24">
+        <v>0</v>
+      </c>
+      <c r="V10" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="33">
+        <v>6</v>
+      </c>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33">
+        <v>6</v>
+      </c>
+      <c r="N11" s="24">
+        <v>0</v>
+      </c>
+      <c r="O11" s="24">
+        <v>0</v>
+      </c>
+      <c r="P11" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="34">
+        <v>3</v>
+      </c>
+      <c r="R11" s="24">
+        <v>0</v>
+      </c>
+      <c r="S11" s="24">
+        <v>0</v>
+      </c>
+      <c r="T11" s="24">
+        <v>0</v>
+      </c>
+      <c r="U11" s="24">
+        <v>0</v>
+      </c>
+      <c r="V11" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="33">
+        <v>7</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33">
+        <v>7</v>
+      </c>
+      <c r="N12" s="24">
+        <v>0</v>
+      </c>
+      <c r="O12" s="24">
+        <v>0</v>
+      </c>
+      <c r="P12" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="34">
+        <v>3</v>
+      </c>
+      <c r="R12" s="24">
+        <v>0</v>
+      </c>
+      <c r="S12" s="24">
+        <v>0</v>
+      </c>
+      <c r="T12" s="24">
+        <v>0</v>
+      </c>
+      <c r="U12" s="24">
+        <v>0</v>
+      </c>
+      <c r="V12" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="33">
+        <v>8</v>
+      </c>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33">
+        <v>8</v>
+      </c>
+      <c r="N13" s="24">
+        <v>0</v>
+      </c>
+      <c r="O13" s="24">
+        <v>0</v>
+      </c>
+      <c r="P13" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="34">
+        <v>3</v>
+      </c>
+      <c r="R13" s="24">
+        <v>0</v>
+      </c>
+      <c r="S13" s="24">
+        <v>0</v>
+      </c>
+      <c r="T13" s="32">
+        <v>0</v>
+      </c>
+      <c r="U13" s="24">
+        <v>0</v>
+      </c>
+      <c r="V13" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="33"/>
+      <c r="O14" s="33"/>
+      <c r="P14" s="33"/>
+      <c r="Q14" s="35"/>
+      <c r="R14" s="33"/>
+      <c r="S14" s="33"/>
+      <c r="T14" s="33"/>
+      <c r="U14" s="33"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI30"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:Z29"/>
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Corrigi o erro de digitação na nova malha
</commit_message>
<xml_diff>
--- a/malhas/malhas-mao-dupla.xlsx
+++ b/malhas/malhas-mao-dupla.xlsx
@@ -6400,7 +6400,7 @@
         <v>3</v>
       </c>
       <c r="AQ16" s="42" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR16" s="42" t="s">
         <v>0</v>
@@ -6598,7 +6598,7 @@
         <v>3</v>
       </c>
       <c r="T18" s="32">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U18" s="32">
         <v>4</v>
@@ -6656,7 +6656,7 @@
         <v>3</v>
       </c>
       <c r="AU18" s="32" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AV18" s="32" t="s">
         <v>1</v>
@@ -6840,7 +6840,7 @@
         <v>2</v>
       </c>
       <c r="P20" s="42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q20" s="28">
         <v>0</v>
@@ -6900,7 +6900,7 @@
         <v>0</v>
       </c>
       <c r="AQ20" s="42" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR20" s="28"/>
       <c r="AS20" s="28"/>

</xml_diff>

<commit_message>
Pequena mudanças na representação da malha
</commit_message>
<xml_diff>
--- a/malhas/malhas-mao-dupla.xlsx
+++ b/malhas/malhas-mao-dupla.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Exemplo1" sheetId="3" r:id="rId1"/>
@@ -174,7 +174,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +277,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -305,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -408,12 +414,11 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1404,14 +1409,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="P15" sqref="P15:Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
     <col min="4" max="4" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
     <col min="6" max="6" width="2.7109375" customWidth="1"/>
@@ -2547,7 +2552,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12" s="1">
         <v>8</v>
@@ -2665,7 +2670,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D13" s="1">
         <v>9</v>
@@ -2783,7 +2788,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D14" s="1">
         <v>10</v>
@@ -2897,11 +2902,11 @@
       <c r="BD14" s="5"/>
     </row>
     <row r="15" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="43">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>32</v>
+      <c r="B15" s="43" t="s">
+        <v>29</v>
       </c>
       <c r="D15" s="1">
         <v>11</v>
@@ -2940,10 +2945,10 @@
         <v>4</v>
       </c>
       <c r="P15" s="20">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="Q15" s="21">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R15" s="19">
         <v>4</v>
@@ -3057,11 +3062,11 @@
       </c>
     </row>
     <row r="16" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="43">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>33</v>
+      <c r="B16" s="43" t="s">
+        <v>32</v>
       </c>
       <c r="D16" s="1">
         <v>12</v>
@@ -3100,7 +3105,7 @@
         <v>2</v>
       </c>
       <c r="P16" s="21">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q16" s="21">
         <v>9</v>
@@ -3217,10 +3222,10 @@
       </c>
     </row>
     <row r="17" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A17" s="26">
+      <c r="A17" s="44">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="43" t="s">
         <v>34</v>
       </c>
       <c r="D17" s="1">
@@ -3335,10 +3340,10 @@
       <c r="BD17" s="5"/>
     </row>
     <row r="18" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="43">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="43" t="s">
         <v>35</v>
       </c>
       <c r="D18" s="1">
@@ -3453,10 +3458,10 @@
       <c r="BD18" s="5"/>
     </row>
     <row r="19" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="43">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="43" t="s">
         <v>36</v>
       </c>
       <c r="D19" s="1">
@@ -3571,10 +3576,10 @@
       <c r="BD19" s="2"/>
     </row>
     <row r="20" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="43">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="43" t="s">
         <v>37</v>
       </c>
       <c r="D20" s="1">
@@ -4746,8 +4751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BF30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:AC29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5721,10 +5726,10 @@
         <v>4</v>
       </c>
       <c r="L11" s="20">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M11" s="21">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N11" s="33">
         <v>4</v>
@@ -5741,10 +5746,10 @@
       <c r="R11" s="33">
         <v>4</v>
       </c>
-      <c r="S11" s="34">
-        <v>14</v>
-      </c>
-      <c r="T11" s="34">
+      <c r="S11" s="20">
+        <v>12</v>
+      </c>
+      <c r="T11" s="21">
         <v>8</v>
       </c>
       <c r="U11" s="33">
@@ -5754,10 +5759,10 @@
         <v>4</v>
       </c>
       <c r="W11" s="20">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="X11" s="21">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y11" s="33">
         <v>4</v>
@@ -5846,7 +5851,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12">
         <v>7</v>
@@ -5873,7 +5878,7 @@
         <v>2</v>
       </c>
       <c r="L12" s="21">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M12" s="21">
         <v>9</v>
@@ -5893,10 +5898,10 @@
       <c r="R12" s="35">
         <v>2</v>
       </c>
-      <c r="S12" s="34">
-        <v>12</v>
-      </c>
-      <c r="T12" s="34">
+      <c r="S12" s="21">
+        <v>11</v>
+      </c>
+      <c r="T12" s="21">
         <v>9</v>
       </c>
       <c r="U12" s="35">
@@ -5906,7 +5911,7 @@
         <v>2</v>
       </c>
       <c r="W12" s="21">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="X12" s="21">
         <v>9</v>
@@ -6000,7 +6005,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D13">
         <v>8</v>
@@ -6126,7 +6131,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D14">
         <v>9</v>
@@ -6248,11 +6253,11 @@
       <c r="BD14" s="28"/>
     </row>
     <row r="15" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="43">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>32</v>
+      <c r="B15" s="43" t="s">
+        <v>29</v>
       </c>
       <c r="D15">
         <v>10</v>
@@ -6299,11 +6304,11 @@
       <c r="R15" s="40">
         <v>4</v>
       </c>
-      <c r="S15" s="34">
-        <v>14</v>
-      </c>
-      <c r="T15" s="34">
-        <v>11</v>
+      <c r="S15" s="20">
+        <v>12</v>
+      </c>
+      <c r="T15" s="21">
+        <v>10</v>
       </c>
       <c r="U15" s="28">
         <v>0</v>
@@ -6378,11 +6383,11 @@
       <c r="BD15" s="28"/>
     </row>
     <row r="16" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="43">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>33</v>
+      <c r="B16" s="43" t="s">
+        <v>32</v>
       </c>
       <c r="D16">
         <v>11</v>
@@ -6429,10 +6434,10 @@
       <c r="R16" s="41">
         <v>2</v>
       </c>
-      <c r="S16" s="34">
-        <v>12</v>
-      </c>
-      <c r="T16" s="34">
+      <c r="S16" s="21">
+        <v>11</v>
+      </c>
+      <c r="T16" s="21">
         <v>5</v>
       </c>
       <c r="U16" s="28">
@@ -6508,10 +6513,10 @@
       <c r="BD16" s="28"/>
     </row>
     <row r="17" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A17" s="26">
+      <c r="A17" s="44">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="43" t="s">
         <v>34</v>
       </c>
       <c r="D17">
@@ -6638,10 +6643,10 @@
       <c r="BD17" s="28"/>
     </row>
     <row r="18" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="43">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="43" t="s">
         <v>35</v>
       </c>
       <c r="D18">
@@ -6772,10 +6777,10 @@
       <c r="BD18" s="28"/>
     </row>
     <row r="19" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="43">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="43" t="s">
         <v>36</v>
       </c>
       <c r="D19">
@@ -6802,11 +6807,11 @@
       <c r="K19" s="28">
         <v>0</v>
       </c>
-      <c r="L19" s="34">
+      <c r="L19" s="20">
         <v>7</v>
       </c>
-      <c r="M19" s="34">
-        <v>11</v>
+      <c r="M19" s="21">
+        <v>10</v>
       </c>
       <c r="N19" s="40">
         <v>4</v>
@@ -6904,10 +6909,10 @@
       <c r="BD19" s="28"/>
     </row>
     <row r="20" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="43">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="43" t="s">
         <v>37</v>
       </c>
       <c r="D20">
@@ -6934,10 +6939,10 @@
       <c r="K20" s="28">
         <v>0</v>
       </c>
-      <c r="L20" s="34">
-        <v>12</v>
-      </c>
-      <c r="M20" s="34">
+      <c r="L20" s="21">
+        <v>11</v>
+      </c>
+      <c r="M20" s="21">
         <v>9</v>
       </c>
       <c r="N20" s="41">
@@ -7272,11 +7277,11 @@
       <c r="K23" s="32">
         <v>4</v>
       </c>
-      <c r="L23" s="42">
-        <v>14</v>
-      </c>
-      <c r="M23" s="34">
-        <v>11</v>
+      <c r="L23" s="20">
+        <v>12</v>
+      </c>
+      <c r="M23" s="21">
+        <v>10</v>
       </c>
       <c r="N23" s="28">
         <v>0</v>
@@ -7373,31 +7378,31 @@
       <c r="D24">
         <v>19</v>
       </c>
-      <c r="E24" s="43">
-        <v>2</v>
-      </c>
-      <c r="F24" s="43">
-        <v>2</v>
-      </c>
-      <c r="G24" s="43">
-        <v>2</v>
-      </c>
-      <c r="H24" s="43">
-        <v>2</v>
-      </c>
-      <c r="I24" s="43">
-        <v>2</v>
-      </c>
-      <c r="J24" s="43">
-        <v>2</v>
-      </c>
-      <c r="K24" s="43">
-        <v>2</v>
-      </c>
-      <c r="L24" s="42">
-        <v>12</v>
-      </c>
-      <c r="M24" s="34">
+      <c r="E24" s="42">
+        <v>2</v>
+      </c>
+      <c r="F24" s="42">
+        <v>2</v>
+      </c>
+      <c r="G24" s="42">
+        <v>2</v>
+      </c>
+      <c r="H24" s="42">
+        <v>2</v>
+      </c>
+      <c r="I24" s="42">
+        <v>2</v>
+      </c>
+      <c r="J24" s="42">
+        <v>2</v>
+      </c>
+      <c r="K24" s="42">
+        <v>2</v>
+      </c>
+      <c r="L24" s="21">
+        <v>11</v>
+      </c>
+      <c r="M24" s="21">
         <v>5</v>
       </c>
       <c r="N24" s="28">
@@ -7451,25 +7456,25 @@
       <c r="AE24">
         <v>19</v>
       </c>
-      <c r="AF24" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG24" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="AH24" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI24" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="AJ24" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK24" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL24" s="43" t="s">
+      <c r="AF24" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG24" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH24" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI24" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK24" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL24" s="42" t="s">
         <v>0</v>
       </c>
       <c r="AM24" s="34"/>

</xml_diff>